<commit_message>
Fixed Standings and totals
</commit_message>
<xml_diff>
--- a/Golf and Bowling Template.xlsx
+++ b/Golf and Bowling Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keens\Documents\GitHub\Golf-Bowling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB5CCDF-60EC-4416-9067-EC10B2D8B116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F7CAD4-F825-452C-8D63-5F967CAA26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{BF288BEB-5C50-45BD-B0E5-559BB8892CD7}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -650,22 +653,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -675,6 +676,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,6 +693,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -697,6 +704,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,16 +728,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5977,34 +5980,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6108,28 +6111,28 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6230,31 +6233,31 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6358,28 +6361,28 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6608,28 +6611,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7135,28 +7138,28 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7257,31 +7260,31 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7385,28 +7388,28 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7510,28 +7513,28 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7635,28 +7638,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8162,28 +8165,28 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8284,31 +8287,31 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8412,28 +8415,28 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8537,28 +8540,28 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8662,28 +8665,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12789,7 +12792,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12939,12 +12942,12 @@
         <v>1</v>
       </c>
       <c r="X2" s="26" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
-        <v>Name #9</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
+        <v>Name #1</v>
       </c>
       <c r="Y2" s="27">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
-        <v>315</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13013,12 +13016,12 @@
         <v>2</v>
       </c>
       <c r="X3" s="28" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
-        <v>Name #8</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
+        <v>Name #2</v>
       </c>
       <c r="Y3" s="19">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
-        <v>297</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13087,12 +13090,12 @@
         <v>3</v>
       </c>
       <c r="X4" s="29" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
-        <v>Name #7</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
+        <v>Name #3</v>
       </c>
       <c r="Y4" s="21">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
-        <v>279</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13161,12 +13164,12 @@
         <v>4</v>
       </c>
       <c r="X5" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
-        <v>Name #6</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
+        <v>Name #4</v>
       </c>
       <c r="Y5" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
-        <v>261</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13235,11 +13238,11 @@
         <v>5</v>
       </c>
       <c r="X6" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
         <v>Name #5</v>
       </c>
       <c r="Y6" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
         <v>243</v>
       </c>
     </row>
@@ -13309,12 +13312,12 @@
         <v>6</v>
       </c>
       <c r="X7" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
-        <v>Name #4</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
+        <v>Name #6</v>
       </c>
       <c r="Y7" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
-        <v>225</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13383,12 +13386,12 @@
         <v>7</v>
       </c>
       <c r="X8" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
-        <v>Name #3</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
+        <v>Name #7</v>
       </c>
       <c r="Y8" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
-        <v>207</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13457,12 +13460,12 @@
         <v>8</v>
       </c>
       <c r="X9" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
-        <v>Name #2</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
+        <v>Name #8</v>
       </c>
       <c r="Y9" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
-        <v>189</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13531,12 +13534,12 @@
         <v>9</v>
       </c>
       <c r="X10" s="10" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
-        <v>Name #1</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
+        <v>Name #9</v>
       </c>
       <c r="Y10" s="12">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
-        <v>171</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -14221,7 +14224,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14372,12 +14375,12 @@
         <v>1</v>
       </c>
       <c r="X2" s="26" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
-        <v>Name #9</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
+        <v>Name #1</v>
       </c>
       <c r="Y2" s="27">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
-        <v>315</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 1), $T$2:$T$10, 0))</f>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14447,12 +14450,12 @@
         <v>2</v>
       </c>
       <c r="X3" s="28" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
-        <v>Name #8</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
+        <v>Name #2</v>
       </c>
       <c r="Y3" s="19">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
-        <v>297</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 2), $T$2:$T$10, 0))</f>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14522,12 +14525,12 @@
         <v>3</v>
       </c>
       <c r="X4" s="29" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
-        <v>Name #7</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
+        <v>Name #3</v>
       </c>
       <c r="Y4" s="21">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
-        <v>279</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 3), $T$2:$T$10, 0))</f>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14597,12 +14600,12 @@
         <v>4</v>
       </c>
       <c r="X5" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
-        <v>Name #6</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
+        <v>Name #4</v>
       </c>
       <c r="Y5" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
-        <v>261</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 4), $T$2:$T$10, 0))</f>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14672,11 +14675,11 @@
         <v>5</v>
       </c>
       <c r="X6" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
         <v>Name #5</v>
       </c>
       <c r="Y6" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 5), $T$2:$T$10, 0))</f>
         <v>243</v>
       </c>
     </row>
@@ -14747,12 +14750,12 @@
         <v>6</v>
       </c>
       <c r="X7" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
-        <v>Name #4</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
+        <v>Name #6</v>
       </c>
       <c r="Y7" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
-        <v>225</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 6), $T$2:$T$10, 0))</f>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14822,12 +14825,12 @@
         <v>7</v>
       </c>
       <c r="X8" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
-        <v>Name #3</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
+        <v>Name #7</v>
       </c>
       <c r="Y8" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
-        <v>207</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 7), $T$2:$T$10, 0))</f>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14897,12 +14900,12 @@
         <v>8</v>
       </c>
       <c r="X9" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
-        <v>Name #2</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
+        <v>Name #8</v>
       </c>
       <c r="Y9" s="9">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
-        <v>189</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 8), $T$2:$T$10, 0))</f>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -14972,12 +14975,12 @@
         <v>9</v>
       </c>
       <c r="X10" s="10" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
-        <v>Name #1</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
+        <v>Name #9</v>
       </c>
       <c r="Y10" s="12">
-        <f>INDEX($T$2:$T$10, MATCH(LARGE($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
-        <v>171</v>
+        <f>INDEX($T$2:$T$10, MATCH(SMALL($T$2:$T$10, 9), $T$2:$T$10, 0))</f>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -15662,7 +15665,7 @@
   <dimension ref="A1:AQ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15957,12 +15960,12 @@
         <v>1</v>
       </c>
       <c r="AP2" s="26" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 1), $AL$2:$AL$10, 0))</f>
-        <v>Name #9</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 1), $AL$2:$AL$10, 0))</f>
+        <v>Name #1</v>
       </c>
       <c r="AQ2" s="27">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 1), $AL$2:$AL$10, 0))</f>
-        <v>630</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 1), $AL$2:$AL$10, 0))</f>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16122,12 +16125,12 @@
         <v>2</v>
       </c>
       <c r="AP3" s="28" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 2), $AL$2:$AL$10, 0))</f>
-        <v>Name #8</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 2), $AL$2:$AL$10, 0))</f>
+        <v>Name #2</v>
       </c>
       <c r="AQ3" s="19">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 2), $AL$2:$AL$10, 0))</f>
-        <v>594</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 2), $AL$2:$AL$10, 0))</f>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16287,12 +16290,12 @@
         <v>3</v>
       </c>
       <c r="AP4" s="29" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 3), $AL$2:$AL$10, 0))</f>
-        <v>Name #7</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 3), $AL$2:$AL$10, 0))</f>
+        <v>Name #3</v>
       </c>
       <c r="AQ4" s="21">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 3), $AL$2:$AL$10, 0))</f>
-        <v>558</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 3), $AL$2:$AL$10, 0))</f>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16452,12 +16455,12 @@
         <v>4</v>
       </c>
       <c r="AP5" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 4), $AL$2:$AL$10, 0))</f>
-        <v>Name #6</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 4), $AL$2:$AL$10, 0))</f>
+        <v>Name #4</v>
       </c>
       <c r="AQ5" s="9">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 4), $AL$2:$AL$10, 0))</f>
-        <v>522</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 4), $AL$2:$AL$10, 0))</f>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16617,11 +16620,11 @@
         <v>5</v>
       </c>
       <c r="AP6" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 5), $AL$2:$AL$10, 0))</f>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 5), $AL$2:$AL$10, 0))</f>
         <v>Name #5</v>
       </c>
       <c r="AQ6" s="9">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 5), $AL$2:$AL$10, 0))</f>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 5), $AL$2:$AL$10, 0))</f>
         <v>486</v>
       </c>
     </row>
@@ -16782,12 +16785,12 @@
         <v>6</v>
       </c>
       <c r="AP7" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 6), $AL$2:$AL$10, 0))</f>
-        <v>Name #4</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 6), $AL$2:$AL$10, 0))</f>
+        <v>Name #6</v>
       </c>
       <c r="AQ7" s="9">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 6), $AL$2:$AL$10, 0))</f>
-        <v>450</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 6), $AL$2:$AL$10, 0))</f>
+        <v>522</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16947,12 +16950,12 @@
         <v>7</v>
       </c>
       <c r="AP8" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 7), $AL$2:$AL$10, 0))</f>
-        <v>Name #3</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 7), $AL$2:$AL$10, 0))</f>
+        <v>Name #7</v>
       </c>
       <c r="AQ8" s="9">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 7), $AL$2:$AL$10, 0))</f>
-        <v>414</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 7), $AL$2:$AL$10, 0))</f>
+        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -17112,12 +17115,12 @@
         <v>8</v>
       </c>
       <c r="AP9" s="7" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 8), $AL$2:$AL$10, 0))</f>
-        <v>Name #2</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 8), $AL$2:$AL$10, 0))</f>
+        <v>Name #8</v>
       </c>
       <c r="AQ9" s="9">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 8), $AL$2:$AL$10, 0))</f>
-        <v>378</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 8), $AL$2:$AL$10, 0))</f>
+        <v>594</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -17277,12 +17280,12 @@
         <v>9</v>
       </c>
       <c r="AP10" s="10" t="str">
-        <f>INDEX($A$2:$A$10, MATCH(LARGE($AL$2:$AL$10, 9), $AL$2:$AL$10, 0))</f>
-        <v>Name #1</v>
+        <f>INDEX($A$2:$A$10, MATCH(SMALL($AL$2:$AL$10, 9), $AL$2:$AL$10, 0))</f>
+        <v>Name #9</v>
       </c>
       <c r="AQ10" s="12">
-        <f>INDEX($AL$2:$AL$10, MATCH(LARGE($AL$2:$AL$10, 9), $AL$2:$AL$10, 0))</f>
-        <v>342</v>
+        <f>INDEX($AL$2:$AL$10, MATCH(SMALL($AL$2:$AL$10, 9), $AL$2:$AL$10, 0))</f>
+        <v>630</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -18615,7 +18618,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="T13" sqref="T13:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18632,47 +18635,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56">
+      <c r="B1" s="62">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="51">
+      <c r="C1" s="58"/>
+      <c r="D1" s="57">
         <v>2</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="51">
+      <c r="E1" s="58"/>
+      <c r="F1" s="57">
         <v>3</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="51">
+      <c r="G1" s="58"/>
+      <c r="H1" s="57">
         <v>4</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="51">
+      <c r="I1" s="58"/>
+      <c r="J1" s="57">
         <v>5</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="51">
+      <c r="K1" s="58"/>
+      <c r="L1" s="57">
         <v>6</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="51">
+      <c r="M1" s="58"/>
+      <c r="N1" s="57">
         <v>7</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="51">
+      <c r="O1" s="58"/>
+      <c r="P1" s="57">
         <v>8</v>
       </c>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="51">
+      <c r="Q1" s="58"/>
+      <c r="R1" s="57">
         <v>9</v>
       </c>
-      <c r="S1" s="52"/>
-      <c r="T1" s="51">
+      <c r="S1" s="58"/>
+      <c r="T1" s="57">
         <v>10</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="54"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="60"/>
       <c r="W1" s="34" t="s">
         <v>1</v>
       </c>
@@ -18687,7 +18690,7 @@
       </c>
     </row>
     <row r="2" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="61" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -18698,107 +18701,139 @@
         <v>14</v>
       </c>
       <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="F2" s="32">
+        <v>4</v>
+      </c>
+      <c r="G2" s="32">
+        <v>4</v>
+      </c>
+      <c r="H2" s="32">
+        <v>4</v>
+      </c>
+      <c r="I2" s="32">
+        <v>4</v>
+      </c>
+      <c r="J2" s="32">
+        <v>4</v>
+      </c>
+      <c r="K2" s="32">
+        <v>4</v>
+      </c>
+      <c r="L2" s="32">
+        <v>4</v>
+      </c>
+      <c r="M2" s="32">
+        <v>4</v>
+      </c>
+      <c r="N2" s="32">
+        <v>4</v>
+      </c>
+      <c r="O2" s="32">
+        <v>4</v>
+      </c>
+      <c r="P2" s="32">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="32">
+        <v>4</v>
+      </c>
+      <c r="R2" s="32">
+        <v>4</v>
+      </c>
+      <c r="S2" s="32">
+        <v>4</v>
+      </c>
+      <c r="T2" s="32">
+        <v>4</v>
+      </c>
+      <c r="U2" s="32">
+        <v>4</v>
+      </c>
       <c r="V2" s="33"/>
-      <c r="W2" s="38">
-        <f>SUM(B3:V3)</f>
-        <v>50</v>
+      <c r="W2" s="51">
+        <f>T3</f>
+        <v>106</v>
       </c>
       <c r="Z2" s="17">
         <v>1</v>
       </c>
       <c r="AA2" s="26" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 1), $W$2:$W$13, 0))</f>
-        <v>Name #5</v>
+        <v>Name #1</v>
       </c>
       <c r="AB2" s="27">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 1), $W$2:$W$13, 0))</f>
-        <v>166</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="35">
+      <c r="A3" s="53"/>
+      <c r="B3" s="55">
         <f>IF(B2&lt;&gt;"",IF(ISERROR(IF(B2="x",IF(AND(D2="x",F2="x"),30,IF(D2="x",20+F2,IF(E2="/",20,10+D2+E2))),IF(AND(C2="/",D2="x"),20,IF(C2="/",10+D2,IF(OR((B2+C2)&gt;9,C2=""),"",B2+C2))))),"",IF(B2="x",IF(AND(D2="x",F2="x"),30,IF(D2="x",20+F2,IF(E2="/",20,10+D2+E2))),IF(AND(C2="/",D2="x"),20,IF(C2="/",10+D2,IF(OR((B2+C2)&gt;9,C2=""),"",B2+C2))))),"")</f>
-        <v>20</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="41">
+        <v>24</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;""),IF(ISERROR(B3+IF(D2="x",IF(AND(F2="x",H2="x"),30,IF(F2="x",20+H2,IF(G2="/",20,10+F2+G2))),IF(AND(E2="/",F2="x"),20,IF(E2="/",10+F2,IF(OR((D2+E2)&gt;9,E2=""),"",D2+E2))))),"",B3+IF(D2="x",IF(AND(F2="x",H2="x"),30,IF(F2="x",20+H2,IF(G2="/",20,10+F2+G2))),IF(AND(E2="/",F2="x"),20,IF(E2="/",10+F2,IF(OR((D2+E2)&gt;9,E2=""),"",D2+E2))))),"")</f>
-        <v>30</v>
-      </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="str">
+        <v>42</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;""),IF(ISERROR(D3+IF(F2="x",IF(AND(H2="x",J2="x"),30,IF(H2="x",20+J2,IF(I2="/",20,10+H2+I2))),IF(AND(G2="/",H2="x"),20,IF(G2="/",10+H2,IF(OR((F2+G2)&gt;9,G2=""),"",F2+G2))))),"",D3+IF(F2="x",IF(AND(H2="x",J2="x"),30,IF(H2="x",20+J2,IF(I2="/",20,10+H2+I2))),IF(AND(G2="/",H2="x"),20,IF(G2="/",10+H2,IF(OR((F2+G2)&gt;9,G2=""),"",F2+G2))))),"")</f>
-        <v/>
-      </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="41" t="str">
+        <v>50</v>
+      </c>
+      <c r="G3" s="44"/>
+      <c r="H3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;""),IF(ISERROR(F3+IF(H2="x",IF(AND(J2="x",L2="x"),30,IF(J2="x",20+L2,IF(K2="/",20,10+J2+K2))),IF(AND(I2="/",J2="x"),20,IF(I2="/",10+J2,IF(OR((H2+I2)&gt;9,I2=""),"",H2+I2))))),"",F3+IF(H2="x",IF(AND(J2="x",L2="x"),30,IF(J2="x",20+L2,IF(K2="/",20,10+J2+K2))),IF(AND(I2="/",J2="x"),20,IF(I2="/",10+J2,IF(OR((H2+I2)&gt;9,I2=""),"",H2+I2))))),"")</f>
-        <v/>
-      </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="41" t="str">
+        <v>58</v>
+      </c>
+      <c r="I3" s="44"/>
+      <c r="J3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;""),IF(ISERROR(H3+IF(J2="x",IF(AND(L2="x",N2="x"),30,IF(L2="x",20+N2,IF(M2="/",20,10+L2+M2))),IF(AND(K2="/",L2="x"),20,IF(K2="/",10+L2,IF(OR((J2+K2)&gt;9,K2=""),"",J2+K2))))),"",H3+IF(J2="x",IF(AND(L2="x",N2="x"),30,IF(L2="x",20+N2,IF(M2="/",20,10+L2+M2))),IF(AND(K2="/",L2="x"),20,IF(K2="/",10+L2,IF(OR((J2+K2)&gt;9,K2=""),"",J2+K2))))),"")</f>
-        <v/>
-      </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="41" t="str">
+        <v>66</v>
+      </c>
+      <c r="K3" s="44"/>
+      <c r="L3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;""),IF(ISERROR(J3+IF(L2="x",IF(AND(N2="x",P2="x"),30,IF(N2="x",20+P2,IF(O2="/",20,10+N2+O2))),IF(AND(M2="/",N2="x"),20,IF(M2="/",10+N2,IF(OR((L2+M2)&gt;9,M2=""),"",L2+M2))))),"",J3+IF(L2="x",IF(AND(N2="x",P2="x"),30,IF(N2="x",20+P2,IF(O2="/",20,10+N2+O2))),IF(AND(M2="/",N2="x"),20,IF(M2="/",10+N2,IF(OR((L2+M2)&gt;9,M2=""),"",L2+M2))))),"")</f>
-        <v/>
-      </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="41" t="str">
+        <v>74</v>
+      </c>
+      <c r="M3" s="44"/>
+      <c r="N3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;""),IF(ISERROR(L3+IF(N2="x",IF(AND(P2="x",R2="x"),30,IF(P2="x",20+R2,IF(Q2="/",20,10+P2+Q2))),IF(AND(O2="/",P2="x"),20,IF(O2="/",10+P2,IF(OR((N2+O2)&gt;9,O2=""),"",N2+O2))))),"",L3+IF(N2="x",IF(AND(P2="x",R2="x"),30,IF(P2="x",20+R2,IF(Q2="/",20,10+P2+Q2))),IF(AND(O2="/",P2="x"),20,IF(O2="/",10+P2,IF(OR((N2+O2)&gt;9,O2=""),"",N2+O2))))),"")</f>
-        <v/>
-      </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="41" t="str">
+        <v>82</v>
+      </c>
+      <c r="O3" s="44"/>
+      <c r="P3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;""),IF(ISERROR(N3+IF(P2="x",IF(AND(R2="x",T2="x"),30,IF(R2="x",20+T2,IF(S2="/",20,10+R2+S2))),IF(AND(Q2="/",R2="x"),20,IF(Q2="/",10+R2,IF(OR((P2+Q2)&gt;9,Q2=""),"",P2+Q2))))),"",N3+IF(P2="x",IF(AND(R2="x",T2="x"),30,IF(R2="x",20+T2,IF(S2="/",20,10+R2+S2))),IF(AND(Q2="/",R2="x"),20,IF(Q2="/",10+R2,IF(OR((P2+Q2)&gt;9,Q2=""),"",P2+Q2))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="41" t="str">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;"",R2&lt;&gt;""),IF(ISERROR(P3+IF(R2="x",IF(AND(T2="x",U2="x"),30,IF(T2="x",20+U2,IF(U2="/",20,10+T2+U2))),IF(AND(S2="/",T2="x"),20,IF(S2="/",10+T2,IF(OR((R2+S2)&gt;9,S2=""),"",R2+S2))))),"",P3+IF(R2="x",IF(AND(T2="x",U2="x"),30,IF(T2="x",20+U2,IF(U2="/",20,10+T2+U2))),IF(AND(S2="/",T2="x"),20,IF(S2="/",10+T2,IF(OR((R2+S2)&gt;9,S2=""),"",R2+S2))))),"")</f>
-        <v/>
-      </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="41" t="str">
+        <v>98</v>
+      </c>
+      <c r="S3" s="44"/>
+      <c r="T3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;"",R2&lt;&gt;"",T2&lt;&gt;""),IF(ISERROR(R3+IF(T2="x",IF(AND(U2="x",V2="x"),30,IF(U2="x",20+V2,IF(V2="/",20,IF(V2&gt;(9-U2),"",10+U2+V2)))),IF(AND(U2="/",V2="x"),20,IF(U2="/",10+V2,IF(OR((T2+U2)&gt;9,U2=""),"",T2+U2))))),"",R3+IF(T2="x",IF(AND(U2="x",V2="x"),30,IF(U2="x",20+V2,IF(V2="/",20,IF(V2&gt;(9-U2),"",10+U2+V2)))),IF(AND(U2="/",V2="x"),20,IF(U2="/",10+V2,IF(OR((T2+U2)&gt;9,U2=""),"",T2+U2))))),"")</f>
-        <v/>
-      </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="39"/>
+        <v>106</v>
+      </c>
+      <c r="U3" s="49"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="42"/>
       <c r="Z3" s="18">
         <v>2</v>
       </c>
       <c r="AA3" s="28" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 2), $W$2:$W$13, 0))</f>
-        <v>Name #1</v>
+        <v>Name #2</v>
       </c>
       <c r="AB3" s="19">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 2), $W$2:$W$13, 0))</f>
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="52" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="7">
@@ -18813,93 +18848,125 @@
       <c r="E4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="F4" s="8">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>3</v>
+      </c>
+      <c r="J4" s="8">
+        <v>3</v>
+      </c>
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8">
+        <v>3</v>
+      </c>
+      <c r="M4" s="8">
+        <v>3</v>
+      </c>
+      <c r="N4" s="8">
+        <v>3</v>
+      </c>
+      <c r="O4" s="8">
+        <v>3</v>
+      </c>
+      <c r="P4" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>3</v>
+      </c>
+      <c r="R4" s="8">
+        <v>3</v>
+      </c>
+      <c r="S4" s="8">
+        <v>3</v>
+      </c>
+      <c r="T4" s="8">
+        <v>3</v>
+      </c>
+      <c r="U4" s="8">
+        <v>3</v>
+      </c>
       <c r="V4" s="9"/>
-      <c r="W4" s="40">
-        <f>SUM(B5:V5)</f>
-        <v>41</v>
+      <c r="W4" s="41">
+        <f>T5</f>
+        <v>73</v>
       </c>
       <c r="Z4" s="20">
         <v>3</v>
       </c>
       <c r="AA4" s="29" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 3), $W$2:$W$13, 0))</f>
-        <v>Name #2</v>
+        <v>Name #6</v>
       </c>
       <c r="AB4" s="21">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 3), $W$2:$W$13, 0))</f>
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="35">
+      <c r="A5" s="53"/>
+      <c r="B5" s="55">
         <f>IF(B4&lt;&gt;"",IF(ISERROR(IF(B4="x",IF(AND(D4="x",F4="x"),30,IF(D4="x",20+F4,IF(E4="/",20,10+D4+E4))),IF(AND(C4="/",D4="x"),20,IF(C4="/",10+D4,IF(OR((B4+C4)&gt;9,C4=""),"",B4+C4))))),"",IF(B4="x",IF(AND(D4="x",F4="x"),30,IF(D4="x",20+F4,IF(E4="/",20,10+D4+E4))),IF(AND(C4="/",D4="x"),20,IF(C4="/",10+D4,IF(OR((B4+C4)&gt;9,C4=""),"",B4+C4))))),"")</f>
         <v>16</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="41">
+      <c r="C5" s="55"/>
+      <c r="D5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;""),IF(ISERROR(B5+IF(D4="x",IF(AND(F4="x",H4="x"),30,IF(F4="x",20+H4,IF(G4="/",20,10+F4+G4))),IF(AND(E4="/",F4="x"),20,IF(E4="/",10+F4,IF(OR((D4+E4)&gt;9,E4=""),"",D4+E4))))),"",B5+IF(D4="x",IF(AND(F4="x",H4="x"),30,IF(F4="x",20+H4,IF(G4="/",20,10+F4+G4))),IF(AND(E4="/",F4="x"),20,IF(E4="/",10+F4,IF(OR((D4+E4)&gt;9,E4=""),"",D4+E4))))),"")</f>
         <v>25</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41" t="str">
+      <c r="E5" s="44"/>
+      <c r="F5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;""),IF(ISERROR(D5+IF(F4="x",IF(AND(H4="x",J4="x"),30,IF(H4="x",20+J4,IF(I4="/",20,10+H4+I4))),IF(AND(G4="/",H4="x"),20,IF(G4="/",10+H4,IF(OR((F4+G4)&gt;9,G4=""),"",F4+G4))))),"",D5+IF(F4="x",IF(AND(H4="x",J4="x"),30,IF(H4="x",20+J4,IF(I4="/",20,10+H4+I4))),IF(AND(G4="/",H4="x"),20,IF(G4="/",10+H4,IF(OR((F4+G4)&gt;9,G4=""),"",F4+G4))))),"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="41" t="str">
+        <v>31</v>
+      </c>
+      <c r="G5" s="44"/>
+      <c r="H5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;""),IF(ISERROR(F5+IF(H4="x",IF(AND(J4="x",L4="x"),30,IF(J4="x",20+L4,IF(K4="/",20,10+J4+K4))),IF(AND(I4="/",J4="x"),20,IF(I4="/",10+J4,IF(OR((H4+I4)&gt;9,I4=""),"",H4+I4))))),"",F5+IF(H4="x",IF(AND(J4="x",L4="x"),30,IF(J4="x",20+L4,IF(K4="/",20,10+J4+K4))),IF(AND(I4="/",J4="x"),20,IF(I4="/",10+J4,IF(OR((H4+I4)&gt;9,I4=""),"",H4+I4))))),"")</f>
-        <v/>
-      </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="41" t="str">
+        <v>37</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;""),IF(ISERROR(H5+IF(J4="x",IF(AND(L4="x",N4="x"),30,IF(L4="x",20+N4,IF(M4="/",20,10+L4+M4))),IF(AND(K4="/",L4="x"),20,IF(K4="/",10+L4,IF(OR((J4+K4)&gt;9,K4=""),"",J4+K4))))),"",H5+IF(J4="x",IF(AND(L4="x",N4="x"),30,IF(L4="x",20+N4,IF(M4="/",20,10+L4+M4))),IF(AND(K4="/",L4="x"),20,IF(K4="/",10+L4,IF(OR((J4+K4)&gt;9,K4=""),"",J4+K4))))),"")</f>
-        <v/>
-      </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="41" t="str">
+        <v>43</v>
+      </c>
+      <c r="K5" s="44"/>
+      <c r="L5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;""),IF(ISERROR(J5+IF(L4="x",IF(AND(N4="x",P4="x"),30,IF(N4="x",20+P4,IF(O4="/",20,10+N4+O4))),IF(AND(M4="/",N4="x"),20,IF(M4="/",10+N4,IF(OR((L4+M4)&gt;9,M4=""),"",L4+M4))))),"",J5+IF(L4="x",IF(AND(N4="x",P4="x"),30,IF(N4="x",20+P4,IF(O4="/",20,10+N4+O4))),IF(AND(M4="/",N4="x"),20,IF(M4="/",10+N4,IF(OR((L4+M4)&gt;9,M4=""),"",L4+M4))))),"")</f>
-        <v/>
-      </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="41" t="str">
+        <v>49</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;""),IF(ISERROR(L5+IF(N4="x",IF(AND(P4="x",R4="x"),30,IF(P4="x",20+R4,IF(Q4="/",20,10+P4+Q4))),IF(AND(O4="/",P4="x"),20,IF(O4="/",10+P4,IF(OR((N4+O4)&gt;9,O4=""),"",N4+O4))))),"",L5+IF(N4="x",IF(AND(P4="x",R4="x"),30,IF(P4="x",20+R4,IF(Q4="/",20,10+P4+Q4))),IF(AND(O4="/",P4="x"),20,IF(O4="/",10+P4,IF(OR((N4+O4)&gt;9,O4=""),"",N4+O4))))),"")</f>
-        <v/>
-      </c>
-      <c r="O5" s="42"/>
-      <c r="P5" s="41" t="str">
+        <v>55</v>
+      </c>
+      <c r="O5" s="44"/>
+      <c r="P5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;""),IF(ISERROR(N5+IF(P4="x",IF(AND(R4="x",T4="x"),30,IF(R4="x",20+T4,IF(S4="/",20,10+R4+S4))),IF(AND(Q4="/",R4="x"),20,IF(Q4="/",10+R4,IF(OR((P4+Q4)&gt;9,Q4=""),"",P4+Q4))))),"",N5+IF(P4="x",IF(AND(R4="x",T4="x"),30,IF(R4="x",20+T4,IF(S4="/",20,10+R4+S4))),IF(AND(Q4="/",R4="x"),20,IF(Q4="/",10+R4,IF(OR((P4+Q4)&gt;9,Q4=""),"",P4+Q4))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="41" t="str">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;"",R4&lt;&gt;""),IF(ISERROR(P5+IF(R4="x",IF(AND(T4="x",U4="x"),30,IF(T4="x",20+U4,IF(U4="/",20,10+T4+U4))),IF(AND(S4="/",T4="x"),20,IF(S4="/",10+T4,IF(OR((R4+S4)&gt;9,S4=""),"",R4+S4))))),"",P5+IF(R4="x",IF(AND(T4="x",U4="x"),30,IF(T4="x",20+U4,IF(U4="/",20,10+T4+U4))),IF(AND(S4="/",T4="x"),20,IF(S4="/",10+T4,IF(OR((R4+S4)&gt;9,S4=""),"",R4+S4))))),"")</f>
-        <v/>
-      </c>
-      <c r="S5" s="42"/>
-      <c r="T5" s="41" t="str">
+        <v>67</v>
+      </c>
+      <c r="S5" s="44"/>
+      <c r="T5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;"",R4&lt;&gt;"",T4&lt;&gt;""),IF(ISERROR(R5+IF(T4="x",IF(AND(U4="x",V4="x"),30,IF(U4="x",20+V4,IF(V4="/",20,IF(V4&gt;(9-U4),"",10+U4+V4)))),IF(AND(U4="/",V4="x"),20,IF(U4="/",10+V4,IF(OR((T4+U4)&gt;9,U4=""),"",T4+U4))))),"",R5+IF(T4="x",IF(AND(U4="x",V4="x"),30,IF(U4="x",20+V4,IF(V4="/",20,IF(V4&gt;(9-U4),"",10+U4+V4)))),IF(AND(U4="/",V4="x"),20,IF(U4="/",10+V4,IF(OR((T4+U4)&gt;9,U4=""),"",T4+U4))))),"")</f>
-        <v/>
-      </c>
-      <c r="U5" s="46"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="39"/>
+        <v>73</v>
+      </c>
+      <c r="U5" s="49"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="42"/>
       <c r="Z5" s="2">
         <v>4</v>
       </c>
@@ -18909,11 +18976,11 @@
       </c>
       <c r="AB5" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 4), $W$2:$W$13, 0))</f>
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="52" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
@@ -18928,26 +18995,58 @@
       <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>2</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2</v>
+      </c>
+      <c r="M6" s="8">
+        <v>2</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2</v>
+      </c>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
+      <c r="P6" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>2</v>
+      </c>
+      <c r="R6" s="8">
+        <v>2</v>
+      </c>
+      <c r="S6" s="8">
+        <v>2</v>
+      </c>
+      <c r="T6" s="8">
+        <v>2</v>
+      </c>
+      <c r="U6" s="8">
+        <v>2</v>
+      </c>
       <c r="V6" s="9"/>
-      <c r="W6" s="40">
-        <f t="shared" ref="W6" si="0">SUM(B7:V7)</f>
-        <v>26</v>
+      <c r="W6" s="41">
+        <f>T7</f>
+        <v>52</v>
       </c>
       <c r="Z6" s="2">
         <v>5</v>
@@ -18958,77 +19057,77 @@
       </c>
       <c r="AB6" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 5), $W$2:$W$13, 0))</f>
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="35">
+      <c r="A7" s="53"/>
+      <c r="B7" s="55">
         <f>IF(B6&lt;&gt;"",IF(ISERROR(IF(B6="x",IF(AND(D6="x",F6="x"),30,IF(D6="x",20+F6,IF(E6="/",20,10+D6+E6))),IF(AND(C6="/",D6="x"),20,IF(C6="/",10+D6,IF(OR((B6+C6)&gt;9,C6=""),"",B6+C6))))),"",IF(B6="x",IF(AND(D6="x",F6="x"),30,IF(D6="x",20+F6,IF(E6="/",20,10+D6+E6))),IF(AND(C6="/",D6="x"),20,IF(C6="/",10+D6,IF(OR((B6+C6)&gt;9,C6=""),"",B6+C6))))),"")</f>
         <v>8</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="41">
+      <c r="C7" s="55"/>
+      <c r="D7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;""),IF(ISERROR(B7+IF(D6="x",IF(AND(F6="x",H6="x"),30,IF(F6="x",20+H6,IF(G6="/",20,10+F6+G6))),IF(AND(E6="/",F6="x"),20,IF(E6="/",10+F6,IF(OR((D6+E6)&gt;9,E6=""),"",D6+E6))))),"",B7+IF(D6="x",IF(AND(F6="x",H6="x"),30,IF(F6="x",20+H6,IF(G6="/",20,10+F6+G6))),IF(AND(E6="/",F6="x"),20,IF(E6="/",10+F6,IF(OR((D6+E6)&gt;9,E6=""),"",D6+E6))))),"")</f>
-        <v>18</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="41" t="str">
+        <v>20</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;""),IF(ISERROR(D7+IF(F6="x",IF(AND(H6="x",J6="x"),30,IF(H6="x",20+J6,IF(I6="/",20,10+H6+I6))),IF(AND(G6="/",H6="x"),20,IF(G6="/",10+H6,IF(OR((F6+G6)&gt;9,G6=""),"",F6+G6))))),"",D7+IF(F6="x",IF(AND(H6="x",J6="x"),30,IF(H6="x",20+J6,IF(I6="/",20,10+H6+I6))),IF(AND(G6="/",H6="x"),20,IF(G6="/",10+H6,IF(OR((F6+G6)&gt;9,G6=""),"",F6+G6))))),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="41" t="str">
+        <v>24</v>
+      </c>
+      <c r="G7" s="44"/>
+      <c r="H7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;""),IF(ISERROR(F7+IF(H6="x",IF(AND(J6="x",L6="x"),30,IF(J6="x",20+L6,IF(K6="/",20,10+J6+K6))),IF(AND(I6="/",J6="x"),20,IF(I6="/",10+J6,IF(OR((H6+I6)&gt;9,I6=""),"",H6+I6))))),"",F7+IF(H6="x",IF(AND(J6="x",L6="x"),30,IF(J6="x",20+L6,IF(K6="/",20,10+J6+K6))),IF(AND(I6="/",J6="x"),20,IF(I6="/",10+J6,IF(OR((H6+I6)&gt;9,I6=""),"",H6+I6))))),"")</f>
-        <v/>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41" t="str">
+        <v>28</v>
+      </c>
+      <c r="I7" s="44"/>
+      <c r="J7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;""),IF(ISERROR(H7+IF(J6="x",IF(AND(L6="x",N6="x"),30,IF(L6="x",20+N6,IF(M6="/",20,10+L6+M6))),IF(AND(K6="/",L6="x"),20,IF(K6="/",10+L6,IF(OR((J6+K6)&gt;9,K6=""),"",J6+K6))))),"",H7+IF(J6="x",IF(AND(L6="x",N6="x"),30,IF(L6="x",20+N6,IF(M6="/",20,10+L6+M6))),IF(AND(K6="/",L6="x"),20,IF(K6="/",10+L6,IF(OR((J6+K6)&gt;9,K6=""),"",J6+K6))))),"")</f>
-        <v/>
-      </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="41" t="str">
+        <v>32</v>
+      </c>
+      <c r="K7" s="44"/>
+      <c r="L7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;""),IF(ISERROR(J7+IF(L6="x",IF(AND(N6="x",P6="x"),30,IF(N6="x",20+P6,IF(O6="/",20,10+N6+O6))),IF(AND(M6="/",N6="x"),20,IF(M6="/",10+N6,IF(OR((L6+M6)&gt;9,M6=""),"",L6+M6))))),"",J7+IF(L6="x",IF(AND(N6="x",P6="x"),30,IF(N6="x",20+P6,IF(O6="/",20,10+N6+O6))),IF(AND(M6="/",N6="x"),20,IF(M6="/",10+N6,IF(OR((L6+M6)&gt;9,M6=""),"",L6+M6))))),"")</f>
-        <v/>
-      </c>
-      <c r="M7" s="42"/>
-      <c r="N7" s="41" t="str">
+        <v>36</v>
+      </c>
+      <c r="M7" s="44"/>
+      <c r="N7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;""),IF(ISERROR(L7+IF(N6="x",IF(AND(P6="x",R6="x"),30,IF(P6="x",20+R6,IF(Q6="/",20,10+P6+Q6))),IF(AND(O6="/",P6="x"),20,IF(O6="/",10+P6,IF(OR((N6+O6)&gt;9,O6=""),"",N6+O6))))),"",L7+IF(N6="x",IF(AND(P6="x",R6="x"),30,IF(P6="x",20+R6,IF(Q6="/",20,10+P6+Q6))),IF(AND(O6="/",P6="x"),20,IF(O6="/",10+P6,IF(OR((N6+O6)&gt;9,O6=""),"",N6+O6))))),"")</f>
-        <v/>
-      </c>
-      <c r="O7" s="42"/>
-      <c r="P7" s="41" t="str">
+        <v>40</v>
+      </c>
+      <c r="O7" s="44"/>
+      <c r="P7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;""),IF(ISERROR(N7+IF(P6="x",IF(AND(R6="x",T6="x"),30,IF(R6="x",20+T6,IF(S6="/",20,10+R6+S6))),IF(AND(Q6="/",R6="x"),20,IF(Q6="/",10+R6,IF(OR((P6+Q6)&gt;9,Q6=""),"",P6+Q6))))),"",N7+IF(P6="x",IF(AND(R6="x",T6="x"),30,IF(R6="x",20+T6,IF(S6="/",20,10+R6+S6))),IF(AND(Q6="/",R6="x"),20,IF(Q6="/",10+R6,IF(OR((P6+Q6)&gt;9,Q6=""),"",P6+Q6))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="41" t="str">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;"",R6&lt;&gt;""),IF(ISERROR(P7+IF(R6="x",IF(AND(T6="x",U6="x"),30,IF(T6="x",20+U6,IF(U6="/",20,10+T6+U6))),IF(AND(S6="/",T6="x"),20,IF(S6="/",10+T6,IF(OR((R6+S6)&gt;9,S6=""),"",R6+S6))))),"",P7+IF(R6="x",IF(AND(T6="x",U6="x"),30,IF(T6="x",20+U6,IF(U6="/",20,10+T6+U6))),IF(AND(S6="/",T6="x"),20,IF(S6="/",10+T6,IF(OR((R6+S6)&gt;9,S6=""),"",R6+S6))))),"")</f>
-        <v/>
-      </c>
-      <c r="S7" s="42"/>
-      <c r="T7" s="41" t="str">
+        <v>48</v>
+      </c>
+      <c r="S7" s="44"/>
+      <c r="T7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;"",R6&lt;&gt;"",T6&lt;&gt;""),IF(ISERROR(R7+IF(T6="x",IF(AND(U6="x",V6="x"),30,IF(U6="x",20+V6,IF(V6="/",20,IF(V6&gt;(9-U6),"",10+U6+V6)))),IF(AND(U6="/",V6="x"),20,IF(U6="/",10+V6,IF(OR((T6+U6)&gt;9,U6=""),"",T6+U6))))),"",R7+IF(T6="x",IF(AND(U6="x",V6="x"),30,IF(U6="x",20+V6,IF(V6="/",20,IF(V6&gt;(9-U6),"",10+U6+V6)))),IF(AND(U6="/",V6="x"),20,IF(U6="/",10+V6,IF(OR((T6+U6)&gt;9,U6=""),"",T6+U6))))),"")</f>
-        <v/>
-      </c>
-      <c r="U7" s="46"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="39"/>
+        <v>52</v>
+      </c>
+      <c r="U7" s="49"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="42"/>
       <c r="Z7" s="2">
         <v>6</v>
       </c>
       <c r="AA7" s="7" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 6), $W$2:$W$13, 0))</f>
-        <v>Name #6</v>
+        <v>Name #5</v>
       </c>
       <c r="AB7" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 6), $W$2:$W$13, 0))</f>
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="52" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7">
@@ -19043,85 +19142,117 @@
       <c r="E8" s="8">
         <v>4</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="8">
+        <v>1</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8">
+        <v>1</v>
+      </c>
       <c r="V8" s="9"/>
-      <c r="W8" s="40">
-        <f t="shared" ref="W8" si="1">SUM(B9:V9)</f>
-        <v>20</v>
+      <c r="W8" s="41">
+        <f>T9</f>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="35">
+      <c r="A9" s="53"/>
+      <c r="B9" s="55">
         <f>IF(B8&lt;&gt;"",IF(ISERROR(IF(B8="x",IF(AND(D8="x",F8="x"),30,IF(D8="x",20+F8,IF(E8="/",20,10+D8+E8))),IF(AND(C8="/",D8="x"),20,IF(C8="/",10+D8,IF(OR((B8+C8)&gt;9,C8=""),"",B8+C8))))),"",IF(B8="x",IF(AND(D8="x",F8="x"),30,IF(D8="x",20+F8,IF(E8="/",20,10+D8+E8))),IF(AND(C8="/",D8="x"),20,IF(C8="/",10+D8,IF(OR((B8+C8)&gt;9,C8=""),"",B8+C8))))),"")</f>
         <v>6</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41">
+      <c r="C9" s="55"/>
+      <c r="D9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;""),IF(ISERROR(B9+IF(D8="x",IF(AND(F8="x",H8="x"),30,IF(F8="x",20+H8,IF(G8="/",20,10+F8+G8))),IF(AND(E8="/",F8="x"),20,IF(E8="/",10+F8,IF(OR((D8+E8)&gt;9,E8=""),"",D8+E8))))),"",B9+IF(D8="x",IF(AND(F8="x",H8="x"),30,IF(F8="x",20+H8,IF(G8="/",20,10+F8+G8))),IF(AND(E8="/",F8="x"),20,IF(E8="/",10+F8,IF(OR((D8+E8)&gt;9,E8=""),"",D8+E8))))),"")</f>
         <v>14</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="41" t="str">
+      <c r="E9" s="44"/>
+      <c r="F9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;""),IF(ISERROR(D9+IF(F8="x",IF(AND(H8="x",J8="x"),30,IF(H8="x",20+J8,IF(I8="/",20,10+H8+I8))),IF(AND(G8="/",H8="x"),20,IF(G8="/",10+H8,IF(OR((F8+G8)&gt;9,G8=""),"",F8+G8))))),"",D9+IF(F8="x",IF(AND(H8="x",J8="x"),30,IF(H8="x",20+J8,IF(I8="/",20,10+H8+I8))),IF(AND(G8="/",H8="x"),20,IF(G8="/",10+H8,IF(OR((F8+G8)&gt;9,G8=""),"",F8+G8))))),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="41" t="str">
+        <v>21</v>
+      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;""),IF(ISERROR(F9+IF(H8="x",IF(AND(J8="x",L8="x"),30,IF(J8="x",20+L8,IF(K8="/",20,10+J8+K8))),IF(AND(I8="/",J8="x"),20,IF(I8="/",10+J8,IF(OR((H8+I8)&gt;9,I8=""),"",H8+I8))))),"",F9+IF(H8="x",IF(AND(J8="x",L8="x"),30,IF(J8="x",20+L8,IF(K8="/",20,10+J8+K8))),IF(AND(I8="/",J8="x"),20,IF(I8="/",10+J8,IF(OR((H8+I8)&gt;9,I8=""),"",H8+I8))))),"")</f>
-        <v/>
-      </c>
-      <c r="I9" s="42"/>
-      <c r="J9" s="41" t="str">
+        <v>26</v>
+      </c>
+      <c r="I9" s="44"/>
+      <c r="J9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;""),IF(ISERROR(H9+IF(J8="x",IF(AND(L8="x",N8="x"),30,IF(L8="x",20+N8,IF(M8="/",20,10+L8+M8))),IF(AND(K8="/",L8="x"),20,IF(K8="/",10+L8,IF(OR((J8+K8)&gt;9,K8=""),"",J8+K8))))),"",H9+IF(J8="x",IF(AND(L8="x",N8="x"),30,IF(L8="x",20+N8,IF(M8="/",20,10+L8+M8))),IF(AND(K8="/",L8="x"),20,IF(K8="/",10+L8,IF(OR((J8+K8)&gt;9,K8=""),"",J8+K8))))),"")</f>
-        <v/>
-      </c>
-      <c r="K9" s="42"/>
-      <c r="L9" s="41" t="str">
+        <v>28</v>
+      </c>
+      <c r="K9" s="44"/>
+      <c r="L9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;""),IF(ISERROR(J9+IF(L8="x",IF(AND(N8="x",P8="x"),30,IF(N8="x",20+P8,IF(O8="/",20,10+N8+O8))),IF(AND(M8="/",N8="x"),20,IF(M8="/",10+N8,IF(OR((L8+M8)&gt;9,M8=""),"",L8+M8))))),"",J9+IF(L8="x",IF(AND(N8="x",P8="x"),30,IF(N8="x",20+P8,IF(O8="/",20,10+N8+O8))),IF(AND(M8="/",N8="x"),20,IF(M8="/",10+N8,IF(OR((L8+M8)&gt;9,M8=""),"",L8+M8))))),"")</f>
-        <v/>
-      </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="41" t="str">
+        <v>30</v>
+      </c>
+      <c r="M9" s="44"/>
+      <c r="N9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;""),IF(ISERROR(L9+IF(N8="x",IF(AND(P8="x",R8="x"),30,IF(P8="x",20+R8,IF(Q8="/",20,10+P8+Q8))),IF(AND(O8="/",P8="x"),20,IF(O8="/",10+P8,IF(OR((N8+O8)&gt;9,O8=""),"",N8+O8))))),"",L9+IF(N8="x",IF(AND(P8="x",R8="x"),30,IF(P8="x",20+R8,IF(Q8="/",20,10+P8+Q8))),IF(AND(O8="/",P8="x"),20,IF(O8="/",10+P8,IF(OR((N8+O8)&gt;9,O8=""),"",N8+O8))))),"")</f>
-        <v/>
-      </c>
-      <c r="O9" s="42"/>
-      <c r="P9" s="41" t="str">
+        <v>32</v>
+      </c>
+      <c r="O9" s="44"/>
+      <c r="P9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;""),IF(ISERROR(N9+IF(P8="x",IF(AND(R8="x",T8="x"),30,IF(R8="x",20+T8,IF(S8="/",20,10+R8+S8))),IF(AND(Q8="/",R8="x"),20,IF(Q8="/",10+R8,IF(OR((P8+Q8)&gt;9,Q8=""),"",P8+Q8))))),"",N9+IF(P8="x",IF(AND(R8="x",T8="x"),30,IF(R8="x",20+T8,IF(S8="/",20,10+R8+S8))),IF(AND(Q8="/",R8="x"),20,IF(Q8="/",10+R8,IF(OR((P8+Q8)&gt;9,Q8=""),"",P8+Q8))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="41" t="str">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;"",R8&lt;&gt;""),IF(ISERROR(P9+IF(R8="x",IF(AND(T8="x",U8="x"),30,IF(T8="x",20+U8,IF(U8="/",20,10+T8+U8))),IF(AND(S8="/",T8="x"),20,IF(S8="/",10+T8,IF(OR((R8+S8)&gt;9,S8=""),"",R8+S8))))),"",P9+IF(R8="x",IF(AND(T8="x",U8="x"),30,IF(T8="x",20+U8,IF(U8="/",20,10+T8+U8))),IF(AND(S8="/",T8="x"),20,IF(S8="/",10+T8,IF(OR((R8+S8)&gt;9,S8=""),"",R8+S8))))),"")</f>
-        <v/>
-      </c>
-      <c r="S9" s="42"/>
-      <c r="T9" s="41" t="str">
+        <v>36</v>
+      </c>
+      <c r="S9" s="44"/>
+      <c r="T9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;"",R8&lt;&gt;"",T8&lt;&gt;""),IF(ISERROR(R9+IF(T8="x",IF(AND(U8="x",V8="x"),30,IF(U8="x",20+V8,IF(V8="/",20,IF(V8&gt;(9-U8),"",10+U8+V8)))),IF(AND(U8="/",V8="x"),20,IF(U8="/",10+V8,IF(OR((T8+U8)&gt;9,U8=""),"",T8+U8))))),"",R9+IF(T8="x",IF(AND(U8="x",V8="x"),30,IF(U8="x",20+V8,IF(V8="/",20,IF(V8&gt;(9-U8),"",10+U8+V8)))),IF(AND(U8="/",V8="x"),20,IF(U8="/",10+V8,IF(OR((T8+U8)&gt;9,U8=""),"",T8+U8))))),"")</f>
-        <v/>
-      </c>
-      <c r="U9" s="46"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="39"/>
+        <v>38</v>
+      </c>
+      <c r="U9" s="49"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="42"/>
     </row>
     <row r="10" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="52" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="7">
@@ -19185,68 +19316,68 @@
         <v>1</v>
       </c>
       <c r="V10" s="9"/>
-      <c r="W10" s="40">
-        <f t="shared" ref="W10" si="2">SUM(B11:V11)</f>
-        <v>166</v>
+      <c r="W10" s="41">
+        <f>T11</f>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="35">
+      <c r="A11" s="53"/>
+      <c r="B11" s="55">
         <f>IF(B10&lt;&gt;"",IF(ISERROR(IF(B10="x",IF(AND(D10="x",F10="x"),30,IF(D10="x",20+F10,IF(E10="/",20,10+D10+E10))),IF(AND(C10="/",D10="x"),20,IF(C10="/",10+D10,IF(OR((B10+C10)&gt;9,C10=""),"",B10+C10))))),"",IF(B10="x",IF(AND(D10="x",F10="x"),30,IF(D10="x",20+F10,IF(E10="/",20,10+D10+E10))),IF(AND(C10="/",D10="x"),20,IF(C10="/",10+D10,IF(OR((B10+C10)&gt;9,C10=""),"",B10+C10))))),"")</f>
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41">
+      <c r="C11" s="55"/>
+      <c r="D11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;""),IF(ISERROR(B11+IF(D10="x",IF(AND(F10="x",H10="x"),30,IF(F10="x",20+H10,IF(G10="/",20,10+F10+G10))),IF(AND(E10="/",F10="x"),20,IF(E10="/",10+F10,IF(OR((D10+E10)&gt;9,E10=""),"",D10+E10))))),"",B11+IF(D10="x",IF(AND(F10="x",H10="x"),30,IF(F10="x",20+H10,IF(G10="/",20,10+F10+G10))),IF(AND(E10="/",F10="x"),20,IF(E10="/",10+F10,IF(OR((D10+E10)&gt;9,E10=""),"",D10+E10))))),"")</f>
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="41">
+      <c r="E11" s="44"/>
+      <c r="F11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;""),IF(ISERROR(D11+IF(F10="x",IF(AND(H10="x",J10="x"),30,IF(H10="x",20+J10,IF(I10="/",20,10+H10+I10))),IF(AND(G10="/",H10="x"),20,IF(G10="/",10+H10,IF(OR((F10+G10)&gt;9,G10=""),"",F10+G10))))),"",D11+IF(F10="x",IF(AND(H10="x",J10="x"),30,IF(H10="x",20+J10,IF(I10="/",20,10+H10+I10))),IF(AND(G10="/",H10="x"),20,IF(G10="/",10+H10,IF(OR((F10+G10)&gt;9,G10=""),"",F10+G10))))),"")</f>
         <v>12</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="41">
+      <c r="G11" s="44"/>
+      <c r="H11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;""),IF(ISERROR(F11+IF(H10="x",IF(AND(J10="x",L10="x"),30,IF(J10="x",20+L10,IF(K10="/",20,10+J10+K10))),IF(AND(I10="/",J10="x"),20,IF(I10="/",10+J10,IF(OR((H10+I10)&gt;9,I10=""),"",H10+I10))))),"",F11+IF(H10="x",IF(AND(J10="x",L10="x"),30,IF(J10="x",20+L10,IF(K10="/",20,10+J10+K10))),IF(AND(I10="/",J10="x"),20,IF(I10="/",10+J10,IF(OR((H10+I10)&gt;9,I10=""),"",H10+I10))))),"")</f>
         <v>14</v>
       </c>
-      <c r="I11" s="42"/>
-      <c r="J11" s="41">
+      <c r="I11" s="44"/>
+      <c r="J11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;""),IF(ISERROR(H11+IF(J10="x",IF(AND(L10="x",N10="x"),30,IF(L10="x",20+N10,IF(M10="/",20,10+L10+M10))),IF(AND(K10="/",L10="x"),20,IF(K10="/",10+L10,IF(OR((J10+K10)&gt;9,K10=""),"",J10+K10))))),"",H11+IF(J10="x",IF(AND(L10="x",N10="x"),30,IF(L10="x",20+N10,IF(M10="/",20,10+L10+M10))),IF(AND(K10="/",L10="x"),20,IF(K10="/",10+L10,IF(OR((J10+K10)&gt;9,K10=""),"",J10+K10))))),"")</f>
         <v>16</v>
       </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="41">
+      <c r="K11" s="44"/>
+      <c r="L11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;""),IF(ISERROR(J11+IF(L10="x",IF(AND(N10="x",P10="x"),30,IF(N10="x",20+P10,IF(O10="/",20,10+N10+O10))),IF(AND(M10="/",N10="x"),20,IF(M10="/",10+N10,IF(OR((L10+M10)&gt;9,M10=""),"",L10+M10))))),"",J11+IF(L10="x",IF(AND(N10="x",P10="x"),30,IF(N10="x",20+P10,IF(O10="/",20,10+N10+O10))),IF(AND(M10="/",N10="x"),20,IF(M10="/",10+N10,IF(OR((L10+M10)&gt;9,M10=""),"",L10+M10))))),"")</f>
         <v>18</v>
       </c>
-      <c r="M11" s="42"/>
-      <c r="N11" s="41">
+      <c r="M11" s="44"/>
+      <c r="N11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;""),IF(ISERROR(L11+IF(N10="x",IF(AND(P10="x",R10="x"),30,IF(P10="x",20+R10,IF(Q10="/",20,10+P10+Q10))),IF(AND(O10="/",P10="x"),20,IF(O10="/",10+P10,IF(OR((N10+O10)&gt;9,O10=""),"",N10+O10))))),"",L11+IF(N10="x",IF(AND(P10="x",R10="x"),30,IF(P10="x",20+R10,IF(Q10="/",20,10+P10+Q10))),IF(AND(O10="/",P10="x"),20,IF(O10="/",10+P10,IF(OR((N10+O10)&gt;9,O10=""),"",N10+O10))))),"")</f>
         <v>20</v>
       </c>
-      <c r="O11" s="42"/>
-      <c r="P11" s="41">
+      <c r="O11" s="44"/>
+      <c r="P11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;""),IF(ISERROR(N11+IF(P10="x",IF(AND(R10="x",T10="x"),30,IF(R10="x",20+T10,IF(S10="/",20,10+R10+S10))),IF(AND(Q10="/",R10="x"),20,IF(Q10="/",10+R10,IF(OR((P10+Q10)&gt;9,Q10=""),"",P10+Q10))))),"",N11+IF(P10="x",IF(AND(R10="x",T10="x"),30,IF(R10="x",20+T10,IF(S10="/",20,10+R10+S10))),IF(AND(Q10="/",R10="x"),20,IF(Q10="/",10+R10,IF(OR((P10+Q10)&gt;9,Q10=""),"",P10+Q10))))),"")</f>
         <v>22</v>
       </c>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="41">
+      <c r="Q11" s="44"/>
+      <c r="R11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;"",R10&lt;&gt;""),IF(ISERROR(P11+IF(R10="x",IF(AND(T10="x",U10="x"),30,IF(T10="x",20+U10,IF(U10="/",20,10+T10+U10))),IF(AND(S10="/",T10="x"),20,IF(S10="/",10+T10,IF(OR((R10+S10)&gt;9,S10=""),"",R10+S10))))),"",P11+IF(R10="x",IF(AND(T10="x",U10="x"),30,IF(T10="x",20+U10,IF(U10="/",20,10+T10+U10))),IF(AND(S10="/",T10="x"),20,IF(S10="/",10+T10,IF(OR((R10+S10)&gt;9,S10=""),"",R10+S10))))),"")</f>
         <v>24</v>
       </c>
-      <c r="S11" s="42"/>
-      <c r="T11" s="41">
+      <c r="S11" s="44"/>
+      <c r="T11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;"",R10&lt;&gt;"",T10&lt;&gt;""),IF(ISERROR(R11+IF(T10="x",IF(AND(U10="x",V10="x"),30,IF(U10="x",20+V10,IF(V10="/",20,IF(V10&gt;(9-U10),"",10+U10+V10)))),IF(AND(U10="/",V10="x"),20,IF(U10="/",10+V10,IF(OR((T10+U10)&gt;9,U10=""),"",T10+U10))))),"",R11+IF(T10="x",IF(AND(U10="x",V10="x"),30,IF(U10="x",20+V10,IF(V10="/",20,IF(V10&gt;(9-U10),"",10+U10+V10)))),IF(AND(U10="/",V10="x"),20,IF(U10="/",10+V10,IF(OR((T10+U10)&gt;9,U10=""),"",T10+U10))))),"")</f>
         <v>26</v>
       </c>
-      <c r="U11" s="46"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="39"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="42"/>
     </row>
     <row r="12" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="52" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="10">
@@ -19261,82 +19392,116 @@
       <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="40">
-        <f>SUM(B13:V13)</f>
-        <v>8</v>
+      <c r="F12" s="8">
+        <v>4</v>
+      </c>
+      <c r="G12" s="8">
+        <v>5</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2</v>
+      </c>
+      <c r="K12" s="8">
+        <v>3</v>
+      </c>
+      <c r="L12" s="8">
+        <v>3</v>
+      </c>
+      <c r="M12" s="8">
+        <v>2</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2</v>
+      </c>
+      <c r="O12" s="8">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>4</v>
+      </c>
+      <c r="R12" s="8">
+        <v>4</v>
+      </c>
+      <c r="S12" s="8">
+        <v>5</v>
+      </c>
+      <c r="T12" s="11">
+        <v>5</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="12">
+        <v>6</v>
+      </c>
+      <c r="W12" s="41">
+        <f>T13</f>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="36">
+      <c r="A13" s="54"/>
+      <c r="B13" s="56">
         <f>IF(B12&lt;&gt;"",IF(ISERROR(IF(B12="x",IF(AND(D12="x",F12="x"),30,IF(D12="x",20+F12,IF(E12="/",20,10+D12+E12))),IF(AND(C12="/",D12="x"),20,IF(C12="/",10+D12,IF(OR((B12+C12)&gt;9,C12=""),"",B12+C12))))),"",IF(B12="x",IF(AND(D12="x",F12="x"),30,IF(D12="x",20+F12,IF(E12="/",20,10+D12+E12))),IF(AND(C12="/",D12="x"),20,IF(C12="/",10+D12,IF(OR((B12+C12)&gt;9,C12=""),"",B12+C12))))),"")</f>
         <v>2</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="43">
+      <c r="C13" s="46"/>
+      <c r="D13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;""),IF(ISERROR(B13+IF(D12="x",IF(AND(F12="x",H12="x"),30,IF(F12="x",20+H12,IF(G12="/",20,10+F12+G12))),IF(AND(E12="/",F12="x"),20,IF(E12="/",10+F12,IF(OR((D12+E12)&gt;9,E12=""),"",D12+E12))))),"",B13+IF(D12="x",IF(AND(F12="x",H12="x"),30,IF(F12="x",20+H12,IF(G12="/",20,10+F12+G12))),IF(AND(E12="/",F12="x"),20,IF(E12="/",10+F12,IF(OR((D12+E12)&gt;9,E12=""),"",D12+E12))))),"")</f>
         <v>6</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="43" t="str">
+      <c r="E13" s="46"/>
+      <c r="F13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;""),IF(ISERROR(D13+IF(F12="x",IF(AND(H12="x",J12="x"),30,IF(H12="x",20+J12,IF(I12="/",20,10+H12+I12))),IF(AND(G12="/",H12="x"),20,IF(G12="/",10+H12,IF(OR((F12+G12)&gt;9,G12=""),"",F12+G12))))),"",D13+IF(F12="x",IF(AND(H12="x",J12="x"),30,IF(H12="x",20+J12,IF(I12="/",20,10+H12+I12))),IF(AND(G12="/",H12="x"),20,IF(G12="/",10+H12,IF(OR((F12+G12)&gt;9,G12=""),"",F12+G12))))),"")</f>
-        <v/>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="43" t="str">
+        <v>15</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;""),IF(ISERROR(F13+IF(H12="x",IF(AND(J12="x",L12="x"),30,IF(J12="x",20+L12,IF(K12="/",20,10+J12+K12))),IF(AND(I12="/",J12="x"),20,IF(I12="/",10+J12,IF(OR((H12+I12)&gt;9,I12=""),"",H12+I12))))),"",F13+IF(H12="x",IF(AND(J12="x",L12="x"),30,IF(J12="x",20+L12,IF(K12="/",20,10+J12+K12))),IF(AND(I12="/",J12="x"),20,IF(I12="/",10+J12,IF(OR((H12+I12)&gt;9,I12=""),"",H12+I12))))),"")</f>
-        <v/>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="43" t="str">
+        <v>22</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;""),IF(ISERROR(H13+IF(J12="x",IF(AND(L12="x",N12="x"),30,IF(L12="x",20+N12,IF(M12="/",20,10+L12+M12))),IF(AND(K12="/",L12="x"),20,IF(K12="/",10+L12,IF(OR((J12+K12)&gt;9,K12=""),"",J12+K12))))),"",H13+IF(J12="x",IF(AND(L12="x",N12="x"),30,IF(L12="x",20+N12,IF(M12="/",20,10+L12+M12))),IF(AND(K12="/",L12="x"),20,IF(K12="/",10+L12,IF(OR((J12+K12)&gt;9,K12=""),"",J12+K12))))),"")</f>
-        <v/>
-      </c>
-      <c r="K13" s="37"/>
-      <c r="L13" s="43" t="str">
+        <v>27</v>
+      </c>
+      <c r="K13" s="46"/>
+      <c r="L13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;""),IF(ISERROR(J13+IF(L12="x",IF(AND(N12="x",P12="x"),30,IF(N12="x",20+P12,IF(O12="/",20,10+N12+O12))),IF(AND(M12="/",N12="x"),20,IF(M12="/",10+N12,IF(OR((L12+M12)&gt;9,M12=""),"",L12+M12))))),"",J13+IF(L12="x",IF(AND(N12="x",P12="x"),30,IF(N12="x",20+P12,IF(O12="/",20,10+N12+O12))),IF(AND(M12="/",N12="x"),20,IF(M12="/",10+N12,IF(OR((L12+M12)&gt;9,M12=""),"",L12+M12))))),"")</f>
-        <v/>
-      </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="43" t="str">
+        <v>32</v>
+      </c>
+      <c r="M13" s="46"/>
+      <c r="N13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;""),IF(ISERROR(L13+IF(N12="x",IF(AND(P12="x",R12="x"),30,IF(P12="x",20+R12,IF(Q12="/",20,10+P12+Q12))),IF(AND(O12="/",P12="x"),20,IF(O12="/",10+P12,IF(OR((N12+O12)&gt;9,O12=""),"",N12+O12))))),"",L13+IF(N12="x",IF(AND(P12="x",R12="x"),30,IF(P12="x",20+R12,IF(Q12="/",20,10+P12+Q12))),IF(AND(O12="/",P12="x"),20,IF(O12="/",10+P12,IF(OR((N12+O12)&gt;9,O12=""),"",N12+O12))))),"")</f>
-        <v/>
-      </c>
-      <c r="O13" s="37"/>
-      <c r="P13" s="43" t="str">
+        <v>36</v>
+      </c>
+      <c r="O13" s="46"/>
+      <c r="P13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;""),IF(ISERROR(N13+IF(P12="x",IF(AND(R12="x",T12="x"),30,IF(R12="x",20+T12,IF(S12="/",20,10+R12+S12))),IF(AND(Q12="/",R12="x"),20,IF(Q12="/",10+R12,IF(OR((P12+Q12)&gt;9,Q12=""),"",P12+Q12))))),"",N13+IF(P12="x",IF(AND(R12="x",T12="x"),30,IF(R12="x",20+T12,IF(S12="/",20,10+R12+S12))),IF(AND(Q12="/",R12="x"),20,IF(Q12="/",10+R12,IF(OR((P12+Q12)&gt;9,Q12=""),"",P12+Q12))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="43" t="str">
+        <v>43</v>
+      </c>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;"",R12&lt;&gt;""),IF(ISERROR(P13+IF(R12="x",IF(AND(T12="x",U12="x"),30,IF(T12="x",20+U12,IF(U12="/",20,10+T12+U12))),IF(AND(S12="/",T12="x"),20,IF(S12="/",10+T12,IF(OR((R12+S12)&gt;9,S12=""),"",R12+S12))))),"",P13+IF(R12="x",IF(AND(T12="x",U12="x"),30,IF(T12="x",20+U12,IF(U12="/",20,10+T12+U12))),IF(AND(S12="/",T12="x"),20,IF(S12="/",10+T12,IF(OR((R12+S12)&gt;9,S12=""),"",R12+S12))))),"")</f>
-        <v/>
-      </c>
-      <c r="S13" s="37"/>
-      <c r="T13" s="43" t="str">
+        <v>52</v>
+      </c>
+      <c r="S13" s="46"/>
+      <c r="T13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;"",R12&lt;&gt;"",T12&lt;&gt;""),IF(ISERROR(R13+IF(T12="x",IF(AND(U12="x",V12="x"),30,IF(U12="x",20+V12,IF(V12="/",20,IF(V12&gt;(9-U12),"",10+U12+V12)))),IF(AND(U12="/",V12="x"),20,IF(U12="/",10+V12,IF(OR((T12+U12)&gt;9,U12=""),"",T12+U12))))),"",R13+IF(T12="x",IF(AND(U12="x",V12="x"),30,IF(U12="x",20+V12,IF(V12="/",20,IF(V12&gt;(9-U12),"",10+U12+V12)))),IF(AND(U12="/",V12="x"),20,IF(U12="/",10+V12,IF(OR((T12+U12)&gt;9,U12=""),"",T12+U12))))),"")</f>
-        <v/>
-      </c>
-      <c r="U13" s="44"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="39"/>
+        <v>68</v>
+      </c>
+      <c r="U13" s="47"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="82">
@@ -19376,6 +19541,8 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F11:G11"/>
@@ -19394,20 +19561,16 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N13:O13"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T5:V5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N13:O13"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="W4:W5"/>
     <mergeCell ref="W6:W7"/>
@@ -19422,6 +19585,8 @@
     <mergeCell ref="T13:V13"/>
     <mergeCell ref="T11:V11"/>
     <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T5:V5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19433,7 +19598,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="T13" sqref="T13:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19450,47 +19615,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56">
+      <c r="B1" s="62">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="51">
+      <c r="C1" s="58"/>
+      <c r="D1" s="57">
         <v>2</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="51">
+      <c r="E1" s="58"/>
+      <c r="F1" s="57">
         <v>3</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="51">
+      <c r="G1" s="58"/>
+      <c r="H1" s="57">
         <v>4</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="51">
+      <c r="I1" s="58"/>
+      <c r="J1" s="57">
         <v>5</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="51">
+      <c r="K1" s="58"/>
+      <c r="L1" s="57">
         <v>6</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="51">
+      <c r="M1" s="58"/>
+      <c r="N1" s="57">
         <v>7</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="51">
+      <c r="O1" s="58"/>
+      <c r="P1" s="57">
         <v>8</v>
       </c>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="51">
+      <c r="Q1" s="58"/>
+      <c r="R1" s="57">
         <v>9</v>
       </c>
-      <c r="S1" s="52"/>
-      <c r="T1" s="51">
+      <c r="S1" s="58"/>
+      <c r="T1" s="57">
         <v>10</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="54"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="60"/>
       <c r="W1" s="34" t="s">
         <v>1</v>
       </c>
@@ -19505,7 +19670,7 @@
       </c>
     </row>
     <row r="2" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="str">
+      <c r="A2" s="61" t="str">
         <f>'Bowling 1'!A2</f>
         <v>Name #1</v>
       </c>
@@ -19570,90 +19735,90 @@
         <v>1</v>
       </c>
       <c r="V2" s="33"/>
-      <c r="W2" s="38">
-        <f>SUM(B3:V3)</f>
-        <v>110</v>
+      <c r="W2" s="51">
+        <f>T3</f>
+        <v>20</v>
       </c>
       <c r="Z2" s="17">
         <v>1</v>
       </c>
       <c r="AA2" s="26" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 1), $W$2:$W$13, 0))</f>
-        <v>Name #1</v>
+        <v>Name #4</v>
       </c>
       <c r="AB2" s="27">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 1), $W$2:$W$13, 0))</f>
-        <v>110</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="35">
+      <c r="A3" s="53"/>
+      <c r="B3" s="55">
         <f>IF(B2&lt;&gt;"",IF(ISERROR(IF(B2="x",IF(AND(D2="x",F2="x"),30,IF(D2="x",20+F2,IF(E2="/",20,10+D2+E2))),IF(AND(C2="/",D2="x"),20,IF(C2="/",10+D2,IF(OR((B2+C2)&gt;9,C2=""),"",B2+C2))))),"",IF(B2="x",IF(AND(D2="x",F2="x"),30,IF(D2="x",20+F2,IF(E2="/",20,10+D2+E2))),IF(AND(C2="/",D2="x"),20,IF(C2="/",10+D2,IF(OR((B2+C2)&gt;9,C2=""),"",B2+C2))))),"")</f>
         <v>2</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="41">
+      <c r="C3" s="55"/>
+      <c r="D3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;""),IF(ISERROR(B3+IF(D2="x",IF(AND(F2="x",H2="x"),30,IF(F2="x",20+H2,IF(G2="/",20,10+F2+G2))),IF(AND(E2="/",F2="x"),20,IF(E2="/",10+F2,IF(OR((D2+E2)&gt;9,E2=""),"",D2+E2))))),"",B3+IF(D2="x",IF(AND(F2="x",H2="x"),30,IF(F2="x",20+H2,IF(G2="/",20,10+F2+G2))),IF(AND(E2="/",F2="x"),20,IF(E2="/",10+F2,IF(OR((D2+E2)&gt;9,E2=""),"",D2+E2))))),"")</f>
         <v>4</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41">
+      <c r="E3" s="44"/>
+      <c r="F3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;""),IF(ISERROR(D3+IF(F2="x",IF(AND(H2="x",J2="x"),30,IF(H2="x",20+J2,IF(I2="/",20,10+H2+I2))),IF(AND(G2="/",H2="x"),20,IF(G2="/",10+H2,IF(OR((F2+G2)&gt;9,G2=""),"",F2+G2))))),"",D3+IF(F2="x",IF(AND(H2="x",J2="x"),30,IF(H2="x",20+J2,IF(I2="/",20,10+H2+I2))),IF(AND(G2="/",H2="x"),20,IF(G2="/",10+H2,IF(OR((F2+G2)&gt;9,G2=""),"",F2+G2))))),"")</f>
         <v>6</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="41">
+      <c r="G3" s="44"/>
+      <c r="H3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;""),IF(ISERROR(F3+IF(H2="x",IF(AND(J2="x",L2="x"),30,IF(J2="x",20+L2,IF(K2="/",20,10+J2+K2))),IF(AND(I2="/",J2="x"),20,IF(I2="/",10+J2,IF(OR((H2+I2)&gt;9,I2=""),"",H2+I2))))),"",F3+IF(H2="x",IF(AND(J2="x",L2="x"),30,IF(J2="x",20+L2,IF(K2="/",20,10+J2+K2))),IF(AND(I2="/",J2="x"),20,IF(I2="/",10+J2,IF(OR((H2+I2)&gt;9,I2=""),"",H2+I2))))),"")</f>
         <v>8</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="41">
+      <c r="I3" s="44"/>
+      <c r="J3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;""),IF(ISERROR(H3+IF(J2="x",IF(AND(L2="x",N2="x"),30,IF(L2="x",20+N2,IF(M2="/",20,10+L2+M2))),IF(AND(K2="/",L2="x"),20,IF(K2="/",10+L2,IF(OR((J2+K2)&gt;9,K2=""),"",J2+K2))))),"",H3+IF(J2="x",IF(AND(L2="x",N2="x"),30,IF(L2="x",20+N2,IF(M2="/",20,10+L2+M2))),IF(AND(K2="/",L2="x"),20,IF(K2="/",10+L2,IF(OR((J2+K2)&gt;9,K2=""),"",J2+K2))))),"")</f>
         <v>10</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="41">
+      <c r="K3" s="44"/>
+      <c r="L3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;""),IF(ISERROR(J3+IF(L2="x",IF(AND(N2="x",P2="x"),30,IF(N2="x",20+P2,IF(O2="/",20,10+N2+O2))),IF(AND(M2="/",N2="x"),20,IF(M2="/",10+N2,IF(OR((L2+M2)&gt;9,M2=""),"",L2+M2))))),"",J3+IF(L2="x",IF(AND(N2="x",P2="x"),30,IF(N2="x",20+P2,IF(O2="/",20,10+N2+O2))),IF(AND(M2="/",N2="x"),20,IF(M2="/",10+N2,IF(OR((L2+M2)&gt;9,M2=""),"",L2+M2))))),"")</f>
         <v>12</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="41">
+      <c r="M3" s="44"/>
+      <c r="N3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;""),IF(ISERROR(L3+IF(N2="x",IF(AND(P2="x",R2="x"),30,IF(P2="x",20+R2,IF(Q2="/",20,10+P2+Q2))),IF(AND(O2="/",P2="x"),20,IF(O2="/",10+P2,IF(OR((N2+O2)&gt;9,O2=""),"",N2+O2))))),"",L3+IF(N2="x",IF(AND(P2="x",R2="x"),30,IF(P2="x",20+R2,IF(Q2="/",20,10+P2+Q2))),IF(AND(O2="/",P2="x"),20,IF(O2="/",10+P2,IF(OR((N2+O2)&gt;9,O2=""),"",N2+O2))))),"")</f>
         <v>14</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="41">
+      <c r="O3" s="44"/>
+      <c r="P3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;""),IF(ISERROR(N3+IF(P2="x",IF(AND(R2="x",T2="x"),30,IF(R2="x",20+T2,IF(S2="/",20,10+R2+S2))),IF(AND(Q2="/",R2="x"),20,IF(Q2="/",10+R2,IF(OR((P2+Q2)&gt;9,Q2=""),"",P2+Q2))))),"",N3+IF(P2="x",IF(AND(R2="x",T2="x"),30,IF(R2="x",20+T2,IF(S2="/",20,10+R2+S2))),IF(AND(Q2="/",R2="x"),20,IF(Q2="/",10+R2,IF(OR((P2+Q2)&gt;9,Q2=""),"",P2+Q2))))),"")</f>
         <v>16</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="41">
+      <c r="Q3" s="44"/>
+      <c r="R3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;"",R2&lt;&gt;""),IF(ISERROR(P3+IF(R2="x",IF(AND(T2="x",U2="x"),30,IF(T2="x",20+U2,IF(U2="/",20,10+T2+U2))),IF(AND(S2="/",T2="x"),20,IF(S2="/",10+T2,IF(OR((R2+S2)&gt;9,S2=""),"",R2+S2))))),"",P3+IF(R2="x",IF(AND(T2="x",U2="x"),30,IF(T2="x",20+U2,IF(U2="/",20,10+T2+U2))),IF(AND(S2="/",T2="x"),20,IF(S2="/",10+T2,IF(OR((R2+S2)&gt;9,S2=""),"",R2+S2))))),"")</f>
         <v>18</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="41">
+      <c r="S3" s="44"/>
+      <c r="T3" s="43">
         <f>IF(AND(B2&lt;&gt;"",D2&lt;&gt;"",F2&lt;&gt;"",H2&lt;&gt;"",J2&lt;&gt;"",L2&lt;&gt;"",N2&lt;&gt;"",P2&lt;&gt;"",R2&lt;&gt;"",T2&lt;&gt;""),IF(ISERROR(R3+IF(T2="x",IF(AND(U2="x",V2="x"),30,IF(U2="x",20+V2,IF(V2="/",20,IF(V2&gt;(9-U2),"",10+U2+V2)))),IF(AND(U2="/",V2="x"),20,IF(U2="/",10+V2,IF(OR((T2+U2)&gt;9,U2=""),"",T2+U2))))),"",R3+IF(T2="x",IF(AND(U2="x",V2="x"),30,IF(U2="x",20+V2,IF(V2="/",20,IF(V2&gt;(9-U2),"",10+U2+V2)))),IF(AND(U2="/",V2="x"),20,IF(U2="/",10+V2,IF(OR((T2+U2)&gt;9,U2=""),"",T2+U2))))),"")</f>
         <v>20</v>
       </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="39"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="42"/>
       <c r="Z3" s="18">
         <v>2</v>
       </c>
       <c r="AA3" s="28" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 2), $W$2:$W$13, 0))</f>
-        <v>Name #2</v>
+        <v>Name #3</v>
       </c>
       <c r="AB3" s="19">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 2), $W$2:$W$13, 0))</f>
-        <v>41</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="str">
+      <c r="A4" s="52" t="str">
         <f>'Bowling 1'!A4</f>
         <v>Name #2</v>
       </c>
@@ -19669,107 +19834,139 @@
       <c r="E4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8">
+        <v>2</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>2</v>
+      </c>
+      <c r="M4" s="8">
+        <v>2</v>
+      </c>
+      <c r="N4" s="8">
+        <v>2</v>
+      </c>
+      <c r="O4" s="8">
+        <v>2</v>
+      </c>
+      <c r="P4" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>2</v>
+      </c>
+      <c r="R4" s="8">
+        <v>2</v>
+      </c>
+      <c r="S4" s="8">
+        <v>2</v>
+      </c>
+      <c r="T4" s="8">
+        <v>2</v>
+      </c>
+      <c r="U4" s="8">
+        <v>2</v>
+      </c>
       <c r="V4" s="9"/>
-      <c r="W4" s="40">
-        <f>SUM(B5:V5)</f>
-        <v>41</v>
+      <c r="W4" s="41">
+        <f>T5</f>
+        <v>57</v>
       </c>
       <c r="Z4" s="20">
         <v>3</v>
       </c>
       <c r="AA4" s="29" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 3), $W$2:$W$13, 0))</f>
-        <v>Name #3</v>
+        <v>Name #6</v>
       </c>
       <c r="AB4" s="21">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 3), $W$2:$W$13, 0))</f>
-        <v>26</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="35">
+      <c r="A5" s="53"/>
+      <c r="B5" s="55">
         <f>IF(B4&lt;&gt;"",IF(ISERROR(IF(B4="x",IF(AND(D4="x",F4="x"),30,IF(D4="x",20+F4,IF(E4="/",20,10+D4+E4))),IF(AND(C4="/",D4="x"),20,IF(C4="/",10+D4,IF(OR((B4+C4)&gt;9,C4=""),"",B4+C4))))),"",IF(B4="x",IF(AND(D4="x",F4="x"),30,IF(D4="x",20+F4,IF(E4="/",20,10+D4+E4))),IF(AND(C4="/",D4="x"),20,IF(C4="/",10+D4,IF(OR((B4+C4)&gt;9,C4=""),"",B4+C4))))),"")</f>
         <v>16</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="41">
+      <c r="C5" s="55"/>
+      <c r="D5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;""),IF(ISERROR(B5+IF(D4="x",IF(AND(F4="x",H4="x"),30,IF(F4="x",20+H4,IF(G4="/",20,10+F4+G4))),IF(AND(E4="/",F4="x"),20,IF(E4="/",10+F4,IF(OR((D4+E4)&gt;9,E4=""),"",D4+E4))))),"",B5+IF(D4="x",IF(AND(F4="x",H4="x"),30,IF(F4="x",20+H4,IF(G4="/",20,10+F4+G4))),IF(AND(E4="/",F4="x"),20,IF(E4="/",10+F4,IF(OR((D4+E4)&gt;9,E4=""),"",D4+E4))))),"")</f>
         <v>25</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41" t="str">
+      <c r="E5" s="44"/>
+      <c r="F5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;""),IF(ISERROR(D5+IF(F4="x",IF(AND(H4="x",J4="x"),30,IF(H4="x",20+J4,IF(I4="/",20,10+H4+I4))),IF(AND(G4="/",H4="x"),20,IF(G4="/",10+H4,IF(OR((F4+G4)&gt;9,G4=""),"",F4+G4))))),"",D5+IF(F4="x",IF(AND(H4="x",J4="x"),30,IF(H4="x",20+J4,IF(I4="/",20,10+H4+I4))),IF(AND(G4="/",H4="x"),20,IF(G4="/",10+H4,IF(OR((F4+G4)&gt;9,G4=""),"",F4+G4))))),"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="41" t="str">
+        <v>29</v>
+      </c>
+      <c r="G5" s="44"/>
+      <c r="H5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;""),IF(ISERROR(F5+IF(H4="x",IF(AND(J4="x",L4="x"),30,IF(J4="x",20+L4,IF(K4="/",20,10+J4+K4))),IF(AND(I4="/",J4="x"),20,IF(I4="/",10+J4,IF(OR((H4+I4)&gt;9,I4=""),"",H4+I4))))),"",F5+IF(H4="x",IF(AND(J4="x",L4="x"),30,IF(J4="x",20+L4,IF(K4="/",20,10+J4+K4))),IF(AND(I4="/",J4="x"),20,IF(I4="/",10+J4,IF(OR((H4+I4)&gt;9,I4=""),"",H4+I4))))),"")</f>
-        <v/>
-      </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="41" t="str">
+        <v>33</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;""),IF(ISERROR(H5+IF(J4="x",IF(AND(L4="x",N4="x"),30,IF(L4="x",20+N4,IF(M4="/",20,10+L4+M4))),IF(AND(K4="/",L4="x"),20,IF(K4="/",10+L4,IF(OR((J4+K4)&gt;9,K4=""),"",J4+K4))))),"",H5+IF(J4="x",IF(AND(L4="x",N4="x"),30,IF(L4="x",20+N4,IF(M4="/",20,10+L4+M4))),IF(AND(K4="/",L4="x"),20,IF(K4="/",10+L4,IF(OR((J4+K4)&gt;9,K4=""),"",J4+K4))))),"")</f>
-        <v/>
-      </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="41" t="str">
+        <v>37</v>
+      </c>
+      <c r="K5" s="44"/>
+      <c r="L5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;""),IF(ISERROR(J5+IF(L4="x",IF(AND(N4="x",P4="x"),30,IF(N4="x",20+P4,IF(O4="/",20,10+N4+O4))),IF(AND(M4="/",N4="x"),20,IF(M4="/",10+N4,IF(OR((L4+M4)&gt;9,M4=""),"",L4+M4))))),"",J5+IF(L4="x",IF(AND(N4="x",P4="x"),30,IF(N4="x",20+P4,IF(O4="/",20,10+N4+O4))),IF(AND(M4="/",N4="x"),20,IF(M4="/",10+N4,IF(OR((L4+M4)&gt;9,M4=""),"",L4+M4))))),"")</f>
-        <v/>
-      </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="41" t="str">
+        <v>41</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;""),IF(ISERROR(L5+IF(N4="x",IF(AND(P4="x",R4="x"),30,IF(P4="x",20+R4,IF(Q4="/",20,10+P4+Q4))),IF(AND(O4="/",P4="x"),20,IF(O4="/",10+P4,IF(OR((N4+O4)&gt;9,O4=""),"",N4+O4))))),"",L5+IF(N4="x",IF(AND(P4="x",R4="x"),30,IF(P4="x",20+R4,IF(Q4="/",20,10+P4+Q4))),IF(AND(O4="/",P4="x"),20,IF(O4="/",10+P4,IF(OR((N4+O4)&gt;9,O4=""),"",N4+O4))))),"")</f>
-        <v/>
-      </c>
-      <c r="O5" s="42"/>
-      <c r="P5" s="41" t="str">
+        <v>45</v>
+      </c>
+      <c r="O5" s="44"/>
+      <c r="P5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;""),IF(ISERROR(N5+IF(P4="x",IF(AND(R4="x",T4="x"),30,IF(R4="x",20+T4,IF(S4="/",20,10+R4+S4))),IF(AND(Q4="/",R4="x"),20,IF(Q4="/",10+R4,IF(OR((P4+Q4)&gt;9,Q4=""),"",P4+Q4))))),"",N5+IF(P4="x",IF(AND(R4="x",T4="x"),30,IF(R4="x",20+T4,IF(S4="/",20,10+R4+S4))),IF(AND(Q4="/",R4="x"),20,IF(Q4="/",10+R4,IF(OR((P4+Q4)&gt;9,Q4=""),"",P4+Q4))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="41" t="str">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;"",R4&lt;&gt;""),IF(ISERROR(P5+IF(R4="x",IF(AND(T4="x",U4="x"),30,IF(T4="x",20+U4,IF(U4="/",20,10+T4+U4))),IF(AND(S4="/",T4="x"),20,IF(S4="/",10+T4,IF(OR((R4+S4)&gt;9,S4=""),"",R4+S4))))),"",P5+IF(R4="x",IF(AND(T4="x",U4="x"),30,IF(T4="x",20+U4,IF(U4="/",20,10+T4+U4))),IF(AND(S4="/",T4="x"),20,IF(S4="/",10+T4,IF(OR((R4+S4)&gt;9,S4=""),"",R4+S4))))),"")</f>
-        <v/>
-      </c>
-      <c r="S5" s="42"/>
-      <c r="T5" s="41" t="str">
+        <v>53</v>
+      </c>
+      <c r="S5" s="44"/>
+      <c r="T5" s="43">
         <f>IF(AND(B4&lt;&gt;"",D4&lt;&gt;"",F4&lt;&gt;"",H4&lt;&gt;"",J4&lt;&gt;"",L4&lt;&gt;"",N4&lt;&gt;"",P4&lt;&gt;"",R4&lt;&gt;"",T4&lt;&gt;""),IF(ISERROR(R5+IF(T4="x",IF(AND(U4="x",V4="x"),30,IF(U4="x",20+V4,IF(V4="/",20,IF(V4&gt;(9-U4),"",10+U4+V4)))),IF(AND(U4="/",V4="x"),20,IF(U4="/",10+V4,IF(OR((T4+U4)&gt;9,U4=""),"",T4+U4))))),"",R5+IF(T4="x",IF(AND(U4="x",V4="x"),30,IF(U4="x",20+V4,IF(V4="/",20,IF(V4&gt;(9-U4),"",10+U4+V4)))),IF(AND(U4="/",V4="x"),20,IF(U4="/",10+V4,IF(OR((T4+U4)&gt;9,U4=""),"",T4+U4))))),"")</f>
-        <v/>
-      </c>
-      <c r="U5" s="46"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="39"/>
+        <v>57</v>
+      </c>
+      <c r="U5" s="49"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="42"/>
       <c r="Z5" s="2">
         <v>4</v>
       </c>
       <c r="AA5" s="7" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 4), $W$2:$W$13, 0))</f>
-        <v>Name #4</v>
+        <v>Name #5</v>
       </c>
       <c r="AB5" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 4), $W$2:$W$13, 0))</f>
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="str">
+      <c r="A6" s="52" t="str">
         <f>'Bowling 1'!A6</f>
         <v>Name #3</v>
       </c>
@@ -19785,107 +19982,139 @@
       <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3</v>
+      </c>
+      <c r="I6" s="8">
+        <v>3</v>
+      </c>
+      <c r="J6" s="8">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3</v>
+      </c>
+      <c r="L6" s="8">
+        <v>3</v>
+      </c>
+      <c r="M6" s="8">
+        <v>3</v>
+      </c>
+      <c r="N6" s="8">
+        <v>3</v>
+      </c>
+      <c r="O6" s="8">
+        <v>3</v>
+      </c>
+      <c r="P6" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>3</v>
+      </c>
+      <c r="R6" s="8">
+        <v>3</v>
+      </c>
+      <c r="S6" s="8">
+        <v>3</v>
+      </c>
+      <c r="T6" s="8">
+        <v>3</v>
+      </c>
+      <c r="U6" s="8">
+        <v>3</v>
+      </c>
       <c r="V6" s="9"/>
-      <c r="W6" s="40">
-        <f t="shared" ref="W6" si="0">SUM(B7:V7)</f>
-        <v>26</v>
+      <c r="W6" s="41">
+        <f>T7</f>
+        <v>69</v>
       </c>
       <c r="Z6" s="2">
         <v>5</v>
       </c>
       <c r="AA6" s="7" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 5), $W$2:$W$13, 0))</f>
-        <v>Name #5</v>
+        <v>Name #2</v>
       </c>
       <c r="AB6" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 5), $W$2:$W$13, 0))</f>
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="35">
+      <c r="A7" s="53"/>
+      <c r="B7" s="55">
         <f>IF(B6&lt;&gt;"",IF(ISERROR(IF(B6="x",IF(AND(D6="x",F6="x"),30,IF(D6="x",20+F6,IF(E6="/",20,10+D6+E6))),IF(AND(C6="/",D6="x"),20,IF(C6="/",10+D6,IF(OR((B6+C6)&gt;9,C6=""),"",B6+C6))))),"",IF(B6="x",IF(AND(D6="x",F6="x"),30,IF(D6="x",20+F6,IF(E6="/",20,10+D6+E6))),IF(AND(C6="/",D6="x"),20,IF(C6="/",10+D6,IF(OR((B6+C6)&gt;9,C6=""),"",B6+C6))))),"")</f>
         <v>8</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="41">
+      <c r="C7" s="55"/>
+      <c r="D7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;""),IF(ISERROR(B7+IF(D6="x",IF(AND(F6="x",H6="x"),30,IF(F6="x",20+H6,IF(G6="/",20,10+F6+G6))),IF(AND(E6="/",F6="x"),20,IF(E6="/",10+F6,IF(OR((D6+E6)&gt;9,E6=""),"",D6+E6))))),"",B7+IF(D6="x",IF(AND(F6="x",H6="x"),30,IF(F6="x",20+H6,IF(G6="/",20,10+F6+G6))),IF(AND(E6="/",F6="x"),20,IF(E6="/",10+F6,IF(OR((D6+E6)&gt;9,E6=""),"",D6+E6))))),"")</f>
-        <v>18</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="41" t="str">
+        <v>21</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;""),IF(ISERROR(D7+IF(F6="x",IF(AND(H6="x",J6="x"),30,IF(H6="x",20+J6,IF(I6="/",20,10+H6+I6))),IF(AND(G6="/",H6="x"),20,IF(G6="/",10+H6,IF(OR((F6+G6)&gt;9,G6=""),"",F6+G6))))),"",D7+IF(F6="x",IF(AND(H6="x",J6="x"),30,IF(H6="x",20+J6,IF(I6="/",20,10+H6+I6))),IF(AND(G6="/",H6="x"),20,IF(G6="/",10+H6,IF(OR((F6+G6)&gt;9,G6=""),"",F6+G6))))),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="41" t="str">
+        <v>27</v>
+      </c>
+      <c r="G7" s="44"/>
+      <c r="H7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;""),IF(ISERROR(F7+IF(H6="x",IF(AND(J6="x",L6="x"),30,IF(J6="x",20+L6,IF(K6="/",20,10+J6+K6))),IF(AND(I6="/",J6="x"),20,IF(I6="/",10+J6,IF(OR((H6+I6)&gt;9,I6=""),"",H6+I6))))),"",F7+IF(H6="x",IF(AND(J6="x",L6="x"),30,IF(J6="x",20+L6,IF(K6="/",20,10+J6+K6))),IF(AND(I6="/",J6="x"),20,IF(I6="/",10+J6,IF(OR((H6+I6)&gt;9,I6=""),"",H6+I6))))),"")</f>
-        <v/>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41" t="str">
+        <v>33</v>
+      </c>
+      <c r="I7" s="44"/>
+      <c r="J7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;""),IF(ISERROR(H7+IF(J6="x",IF(AND(L6="x",N6="x"),30,IF(L6="x",20+N6,IF(M6="/",20,10+L6+M6))),IF(AND(K6="/",L6="x"),20,IF(K6="/",10+L6,IF(OR((J6+K6)&gt;9,K6=""),"",J6+K6))))),"",H7+IF(J6="x",IF(AND(L6="x",N6="x"),30,IF(L6="x",20+N6,IF(M6="/",20,10+L6+M6))),IF(AND(K6="/",L6="x"),20,IF(K6="/",10+L6,IF(OR((J6+K6)&gt;9,K6=""),"",J6+K6))))),"")</f>
-        <v/>
-      </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="41" t="str">
+        <v>39</v>
+      </c>
+      <c r="K7" s="44"/>
+      <c r="L7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;""),IF(ISERROR(J7+IF(L6="x",IF(AND(N6="x",P6="x"),30,IF(N6="x",20+P6,IF(O6="/",20,10+N6+O6))),IF(AND(M6="/",N6="x"),20,IF(M6="/",10+N6,IF(OR((L6+M6)&gt;9,M6=""),"",L6+M6))))),"",J7+IF(L6="x",IF(AND(N6="x",P6="x"),30,IF(N6="x",20+P6,IF(O6="/",20,10+N6+O6))),IF(AND(M6="/",N6="x"),20,IF(M6="/",10+N6,IF(OR((L6+M6)&gt;9,M6=""),"",L6+M6))))),"")</f>
-        <v/>
-      </c>
-      <c r="M7" s="42"/>
-      <c r="N7" s="41" t="str">
+        <v>45</v>
+      </c>
+      <c r="M7" s="44"/>
+      <c r="N7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;""),IF(ISERROR(L7+IF(N6="x",IF(AND(P6="x",R6="x"),30,IF(P6="x",20+R6,IF(Q6="/",20,10+P6+Q6))),IF(AND(O6="/",P6="x"),20,IF(O6="/",10+P6,IF(OR((N6+O6)&gt;9,O6=""),"",N6+O6))))),"",L7+IF(N6="x",IF(AND(P6="x",R6="x"),30,IF(P6="x",20+R6,IF(Q6="/",20,10+P6+Q6))),IF(AND(O6="/",P6="x"),20,IF(O6="/",10+P6,IF(OR((N6+O6)&gt;9,O6=""),"",N6+O6))))),"")</f>
-        <v/>
-      </c>
-      <c r="O7" s="42"/>
-      <c r="P7" s="41" t="str">
+        <v>51</v>
+      </c>
+      <c r="O7" s="44"/>
+      <c r="P7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;""),IF(ISERROR(N7+IF(P6="x",IF(AND(R6="x",T6="x"),30,IF(R6="x",20+T6,IF(S6="/",20,10+R6+S6))),IF(AND(Q6="/",R6="x"),20,IF(Q6="/",10+R6,IF(OR((P6+Q6)&gt;9,Q6=""),"",P6+Q6))))),"",N7+IF(P6="x",IF(AND(R6="x",T6="x"),30,IF(R6="x",20+T6,IF(S6="/",20,10+R6+S6))),IF(AND(Q6="/",R6="x"),20,IF(Q6="/",10+R6,IF(OR((P6+Q6)&gt;9,Q6=""),"",P6+Q6))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="41" t="str">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;"",R6&lt;&gt;""),IF(ISERROR(P7+IF(R6="x",IF(AND(T6="x",U6="x"),30,IF(T6="x",20+U6,IF(U6="/",20,10+T6+U6))),IF(AND(S6="/",T6="x"),20,IF(S6="/",10+T6,IF(OR((R6+S6)&gt;9,S6=""),"",R6+S6))))),"",P7+IF(R6="x",IF(AND(T6="x",U6="x"),30,IF(T6="x",20+U6,IF(U6="/",20,10+T6+U6))),IF(AND(S6="/",T6="x"),20,IF(S6="/",10+T6,IF(OR((R6+S6)&gt;9,S6=""),"",R6+S6))))),"")</f>
-        <v/>
-      </c>
-      <c r="S7" s="42"/>
-      <c r="T7" s="41" t="str">
+        <v>63</v>
+      </c>
+      <c r="S7" s="44"/>
+      <c r="T7" s="43">
         <f>IF(AND(B6&lt;&gt;"",D6&lt;&gt;"",F6&lt;&gt;"",H6&lt;&gt;"",J6&lt;&gt;"",L6&lt;&gt;"",N6&lt;&gt;"",P6&lt;&gt;"",R6&lt;&gt;"",T6&lt;&gt;""),IF(ISERROR(R7+IF(T6="x",IF(AND(U6="x",V6="x"),30,IF(U6="x",20+V6,IF(V6="/",20,IF(V6&gt;(9-U6),"",10+U6+V6)))),IF(AND(U6="/",V6="x"),20,IF(U6="/",10+V6,IF(OR((T6+U6)&gt;9,U6=""),"",T6+U6))))),"",R7+IF(T6="x",IF(AND(U6="x",V6="x"),30,IF(U6="x",20+V6,IF(V6="/",20,IF(V6&gt;(9-U6),"",10+U6+V6)))),IF(AND(U6="/",V6="x"),20,IF(U6="/",10+V6,IF(OR((T6+U6)&gt;9,U6=""),"",T6+U6))))),"")</f>
-        <v/>
-      </c>
-      <c r="U7" s="46"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="39"/>
+        <v>69</v>
+      </c>
+      <c r="U7" s="49"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="42"/>
       <c r="Z7" s="2">
         <v>6</v>
       </c>
       <c r="AA7" s="7" t="str">
         <f>INDEX($A$2:$A$13, MATCH(LARGE($W$2:$W$13, 6), $W$2:$W$13, 0))</f>
-        <v>Name #6</v>
+        <v>Name #1</v>
       </c>
       <c r="AB7" s="9">
         <f>INDEX($W$2:$W$13, MATCH(LARGE($W$2:$W$13, 6), $W$2:$W$13, 0))</f>
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="str">
+      <c r="A8" s="52" t="str">
         <f>'Bowling 1'!A8</f>
         <v>Name #4</v>
       </c>
@@ -19901,85 +20130,117 @@
       <c r="E8" s="8">
         <v>4</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4</v>
+      </c>
+      <c r="K8" s="8">
+        <v>4</v>
+      </c>
+      <c r="L8" s="8">
+        <v>4</v>
+      </c>
+      <c r="M8" s="8">
+        <v>4</v>
+      </c>
+      <c r="N8" s="8">
+        <v>4</v>
+      </c>
+      <c r="O8" s="8">
+        <v>4</v>
+      </c>
+      <c r="P8" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>4</v>
+      </c>
+      <c r="R8" s="8">
+        <v>4</v>
+      </c>
+      <c r="S8" s="8">
+        <v>4</v>
+      </c>
+      <c r="T8" s="8">
+        <v>4</v>
+      </c>
+      <c r="U8" s="8">
+        <v>4</v>
+      </c>
       <c r="V8" s="9"/>
-      <c r="W8" s="40">
-        <f t="shared" ref="W8" si="1">SUM(B9:V9)</f>
-        <v>20</v>
+      <c r="W8" s="41">
+        <f>T9</f>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="35">
+      <c r="A9" s="53"/>
+      <c r="B9" s="55">
         <f>IF(B8&lt;&gt;"",IF(ISERROR(IF(B8="x",IF(AND(D8="x",F8="x"),30,IF(D8="x",20+F8,IF(E8="/",20,10+D8+E8))),IF(AND(C8="/",D8="x"),20,IF(C8="/",10+D8,IF(OR((B8+C8)&gt;9,C8=""),"",B8+C8))))),"",IF(B8="x",IF(AND(D8="x",F8="x"),30,IF(D8="x",20+F8,IF(E8="/",20,10+D8+E8))),IF(AND(C8="/",D8="x"),20,IF(C8="/",10+D8,IF(OR((B8+C8)&gt;9,C8=""),"",B8+C8))))),"")</f>
         <v>6</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41">
+      <c r="C9" s="55"/>
+      <c r="D9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;""),IF(ISERROR(B9+IF(D8="x",IF(AND(F8="x",H8="x"),30,IF(F8="x",20+H8,IF(G8="/",20,10+F8+G8))),IF(AND(E8="/",F8="x"),20,IF(E8="/",10+F8,IF(OR((D8+E8)&gt;9,E8=""),"",D8+E8))))),"",B9+IF(D8="x",IF(AND(F8="x",H8="x"),30,IF(F8="x",20+H8,IF(G8="/",20,10+F8+G8))),IF(AND(E8="/",F8="x"),20,IF(E8="/",10+F8,IF(OR((D8+E8)&gt;9,E8=""),"",D8+E8))))),"")</f>
         <v>14</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="41" t="str">
+      <c r="E9" s="44"/>
+      <c r="F9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;""),IF(ISERROR(D9+IF(F8="x",IF(AND(H8="x",J8="x"),30,IF(H8="x",20+J8,IF(I8="/",20,10+H8+I8))),IF(AND(G8="/",H8="x"),20,IF(G8="/",10+H8,IF(OR((F8+G8)&gt;9,G8=""),"",F8+G8))))),"",D9+IF(F8="x",IF(AND(H8="x",J8="x"),30,IF(H8="x",20+J8,IF(I8="/",20,10+H8+I8))),IF(AND(G8="/",H8="x"),20,IF(G8="/",10+H8,IF(OR((F8+G8)&gt;9,G8=""),"",F8+G8))))),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="41" t="str">
+        <v>22</v>
+      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;""),IF(ISERROR(F9+IF(H8="x",IF(AND(J8="x",L8="x"),30,IF(J8="x",20+L8,IF(K8="/",20,10+J8+K8))),IF(AND(I8="/",J8="x"),20,IF(I8="/",10+J8,IF(OR((H8+I8)&gt;9,I8=""),"",H8+I8))))),"",F9+IF(H8="x",IF(AND(J8="x",L8="x"),30,IF(J8="x",20+L8,IF(K8="/",20,10+J8+K8))),IF(AND(I8="/",J8="x"),20,IF(I8="/",10+J8,IF(OR((H8+I8)&gt;9,I8=""),"",H8+I8))))),"")</f>
-        <v/>
-      </c>
-      <c r="I9" s="42"/>
-      <c r="J9" s="41" t="str">
+        <v>30</v>
+      </c>
+      <c r="I9" s="44"/>
+      <c r="J9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;""),IF(ISERROR(H9+IF(J8="x",IF(AND(L8="x",N8="x"),30,IF(L8="x",20+N8,IF(M8="/",20,10+L8+M8))),IF(AND(K8="/",L8="x"),20,IF(K8="/",10+L8,IF(OR((J8+K8)&gt;9,K8=""),"",J8+K8))))),"",H9+IF(J8="x",IF(AND(L8="x",N8="x"),30,IF(L8="x",20+N8,IF(M8="/",20,10+L8+M8))),IF(AND(K8="/",L8="x"),20,IF(K8="/",10+L8,IF(OR((J8+K8)&gt;9,K8=""),"",J8+K8))))),"")</f>
-        <v/>
-      </c>
-      <c r="K9" s="42"/>
-      <c r="L9" s="41" t="str">
+        <v>38</v>
+      </c>
+      <c r="K9" s="44"/>
+      <c r="L9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;""),IF(ISERROR(J9+IF(L8="x",IF(AND(N8="x",P8="x"),30,IF(N8="x",20+P8,IF(O8="/",20,10+N8+O8))),IF(AND(M8="/",N8="x"),20,IF(M8="/",10+N8,IF(OR((L8+M8)&gt;9,M8=""),"",L8+M8))))),"",J9+IF(L8="x",IF(AND(N8="x",P8="x"),30,IF(N8="x",20+P8,IF(O8="/",20,10+N8+O8))),IF(AND(M8="/",N8="x"),20,IF(M8="/",10+N8,IF(OR((L8+M8)&gt;9,M8=""),"",L8+M8))))),"")</f>
-        <v/>
-      </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="41" t="str">
+        <v>46</v>
+      </c>
+      <c r="M9" s="44"/>
+      <c r="N9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;""),IF(ISERROR(L9+IF(N8="x",IF(AND(P8="x",R8="x"),30,IF(P8="x",20+R8,IF(Q8="/",20,10+P8+Q8))),IF(AND(O8="/",P8="x"),20,IF(O8="/",10+P8,IF(OR((N8+O8)&gt;9,O8=""),"",N8+O8))))),"",L9+IF(N8="x",IF(AND(P8="x",R8="x"),30,IF(P8="x",20+R8,IF(Q8="/",20,10+P8+Q8))),IF(AND(O8="/",P8="x"),20,IF(O8="/",10+P8,IF(OR((N8+O8)&gt;9,O8=""),"",N8+O8))))),"")</f>
-        <v/>
-      </c>
-      <c r="O9" s="42"/>
-      <c r="P9" s="41" t="str">
+        <v>54</v>
+      </c>
+      <c r="O9" s="44"/>
+      <c r="P9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;""),IF(ISERROR(N9+IF(P8="x",IF(AND(R8="x",T8="x"),30,IF(R8="x",20+T8,IF(S8="/",20,10+R8+S8))),IF(AND(Q8="/",R8="x"),20,IF(Q8="/",10+R8,IF(OR((P8+Q8)&gt;9,Q8=""),"",P8+Q8))))),"",N9+IF(P8="x",IF(AND(R8="x",T8="x"),30,IF(R8="x",20+T8,IF(S8="/",20,10+R8+S8))),IF(AND(Q8="/",R8="x"),20,IF(Q8="/",10+R8,IF(OR((P8+Q8)&gt;9,Q8=""),"",P8+Q8))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="41" t="str">
+        <v>62</v>
+      </c>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;"",R8&lt;&gt;""),IF(ISERROR(P9+IF(R8="x",IF(AND(T8="x",U8="x"),30,IF(T8="x",20+U8,IF(U8="/",20,10+T8+U8))),IF(AND(S8="/",T8="x"),20,IF(S8="/",10+T8,IF(OR((R8+S8)&gt;9,S8=""),"",R8+S8))))),"",P9+IF(R8="x",IF(AND(T8="x",U8="x"),30,IF(T8="x",20+U8,IF(U8="/",20,10+T8+U8))),IF(AND(S8="/",T8="x"),20,IF(S8="/",10+T8,IF(OR((R8+S8)&gt;9,S8=""),"",R8+S8))))),"")</f>
-        <v/>
-      </c>
-      <c r="S9" s="42"/>
-      <c r="T9" s="41" t="str">
+        <v>70</v>
+      </c>
+      <c r="S9" s="44"/>
+      <c r="T9" s="43">
         <f>IF(AND(B8&lt;&gt;"",D8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",L8&lt;&gt;"",N8&lt;&gt;"",P8&lt;&gt;"",R8&lt;&gt;"",T8&lt;&gt;""),IF(ISERROR(R9+IF(T8="x",IF(AND(U8="x",V8="x"),30,IF(U8="x",20+V8,IF(V8="/",20,IF(V8&gt;(9-U8),"",10+U8+V8)))),IF(AND(U8="/",V8="x"),20,IF(U8="/",10+V8,IF(OR((T8+U8)&gt;9,U8=""),"",T8+U8))))),"",R9+IF(T8="x",IF(AND(U8="x",V8="x"),30,IF(U8="x",20+V8,IF(V8="/",20,IF(V8&gt;(9-U8),"",10+U8+V8)))),IF(AND(U8="/",V8="x"),20,IF(U8="/",10+V8,IF(OR((T8+U8)&gt;9,U8=""),"",T8+U8))))),"")</f>
-        <v/>
-      </c>
-      <c r="U9" s="46"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="39"/>
+        <v>78</v>
+      </c>
+      <c r="U9" s="49"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="42"/>
     </row>
     <row r="10" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="str">
+      <c r="A10" s="52" t="str">
         <f>'Bowling 1'!A10</f>
         <v>Name #5</v>
       </c>
@@ -19995,85 +20256,117 @@
       <c r="E10" s="8">
         <v>3</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3</v>
+      </c>
+      <c r="H10" s="8">
+        <v>3</v>
+      </c>
+      <c r="I10" s="8">
+        <v>3</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3</v>
+      </c>
+      <c r="K10" s="8">
+        <v>3</v>
+      </c>
+      <c r="L10" s="8">
+        <v>3</v>
+      </c>
+      <c r="M10" s="8">
+        <v>3</v>
+      </c>
+      <c r="N10" s="8">
+        <v>3</v>
+      </c>
+      <c r="O10" s="8">
+        <v>3</v>
+      </c>
+      <c r="P10" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>3</v>
+      </c>
+      <c r="R10" s="8">
+        <v>3</v>
+      </c>
+      <c r="S10" s="8">
+        <v>3</v>
+      </c>
+      <c r="T10" s="8">
+        <v>3</v>
+      </c>
+      <c r="U10" s="8">
+        <v>3</v>
+      </c>
       <c r="V10" s="9"/>
-      <c r="W10" s="40">
-        <f t="shared" ref="W10" si="2">SUM(B11:V11)</f>
-        <v>14</v>
+      <c r="W10" s="41">
+        <f>T11</f>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="35">
+      <c r="A11" s="53"/>
+      <c r="B11" s="55">
         <f>IF(B10&lt;&gt;"",IF(ISERROR(IF(B10="x",IF(AND(D10="x",F10="x"),30,IF(D10="x",20+F10,IF(E10="/",20,10+D10+E10))),IF(AND(C10="/",D10="x"),20,IF(C10="/",10+D10,IF(OR((B10+C10)&gt;9,C10=""),"",B10+C10))))),"",IF(B10="x",IF(AND(D10="x",F10="x"),30,IF(D10="x",20+F10,IF(E10="/",20,10+D10+E10))),IF(AND(C10="/",D10="x"),20,IF(C10="/",10+D10,IF(OR((B10+C10)&gt;9,C10=""),"",B10+C10))))),"")</f>
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41">
+      <c r="C11" s="55"/>
+      <c r="D11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;""),IF(ISERROR(B11+IF(D10="x",IF(AND(F10="x",H10="x"),30,IF(F10="x",20+H10,IF(G10="/",20,10+F10+G10))),IF(AND(E10="/",F10="x"),20,IF(E10="/",10+F10,IF(OR((D10+E10)&gt;9,E10=""),"",D10+E10))))),"",B11+IF(D10="x",IF(AND(F10="x",H10="x"),30,IF(F10="x",20+H10,IF(G10="/",20,10+F10+G10))),IF(AND(E10="/",F10="x"),20,IF(E10="/",10+F10,IF(OR((D10+E10)&gt;9,E10=""),"",D10+E10))))),"")</f>
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="41" t="str">
+      <c r="E11" s="44"/>
+      <c r="F11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;""),IF(ISERROR(D11+IF(F10="x",IF(AND(H10="x",J10="x"),30,IF(H10="x",20+J10,IF(I10="/",20,10+H10+I10))),IF(AND(G10="/",H10="x"),20,IF(G10="/",10+H10,IF(OR((F10+G10)&gt;9,G10=""),"",F10+G10))))),"",D11+IF(F10="x",IF(AND(H10="x",J10="x"),30,IF(H10="x",20+J10,IF(I10="/",20,10+H10+I10))),IF(AND(G10="/",H10="x"),20,IF(G10="/",10+H10,IF(OR((F10+G10)&gt;9,G10=""),"",F10+G10))))),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="41" t="str">
+        <v>16</v>
+      </c>
+      <c r="G11" s="44"/>
+      <c r="H11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;""),IF(ISERROR(F11+IF(H10="x",IF(AND(J10="x",L10="x"),30,IF(J10="x",20+L10,IF(K10="/",20,10+J10+K10))),IF(AND(I10="/",J10="x"),20,IF(I10="/",10+J10,IF(OR((H10+I10)&gt;9,I10=""),"",H10+I10))))),"",F11+IF(H10="x",IF(AND(J10="x",L10="x"),30,IF(J10="x",20+L10,IF(K10="/",20,10+J10+K10))),IF(AND(I10="/",J10="x"),20,IF(I10="/",10+J10,IF(OR((H10+I10)&gt;9,I10=""),"",H10+I10))))),"")</f>
-        <v/>
-      </c>
-      <c r="I11" s="42"/>
-      <c r="J11" s="41" t="str">
+        <v>22</v>
+      </c>
+      <c r="I11" s="44"/>
+      <c r="J11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;""),IF(ISERROR(H11+IF(J10="x",IF(AND(L10="x",N10="x"),30,IF(L10="x",20+N10,IF(M10="/",20,10+L10+M10))),IF(AND(K10="/",L10="x"),20,IF(K10="/",10+L10,IF(OR((J10+K10)&gt;9,K10=""),"",J10+K10))))),"",H11+IF(J10="x",IF(AND(L10="x",N10="x"),30,IF(L10="x",20+N10,IF(M10="/",20,10+L10+M10))),IF(AND(K10="/",L10="x"),20,IF(K10="/",10+L10,IF(OR((J10+K10)&gt;9,K10=""),"",J10+K10))))),"")</f>
-        <v/>
-      </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="41" t="str">
+        <v>28</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;""),IF(ISERROR(J11+IF(L10="x",IF(AND(N10="x",P10="x"),30,IF(N10="x",20+P10,IF(O10="/",20,10+N10+O10))),IF(AND(M10="/",N10="x"),20,IF(M10="/",10+N10,IF(OR((L10+M10)&gt;9,M10=""),"",L10+M10))))),"",J11+IF(L10="x",IF(AND(N10="x",P10="x"),30,IF(N10="x",20+P10,IF(O10="/",20,10+N10+O10))),IF(AND(M10="/",N10="x"),20,IF(M10="/",10+N10,IF(OR((L10+M10)&gt;9,M10=""),"",L10+M10))))),"")</f>
-        <v/>
-      </c>
-      <c r="M11" s="42"/>
-      <c r="N11" s="41" t="str">
+        <v>34</v>
+      </c>
+      <c r="M11" s="44"/>
+      <c r="N11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;""),IF(ISERROR(L11+IF(N10="x",IF(AND(P10="x",R10="x"),30,IF(P10="x",20+R10,IF(Q10="/",20,10+P10+Q10))),IF(AND(O10="/",P10="x"),20,IF(O10="/",10+P10,IF(OR((N10+O10)&gt;9,O10=""),"",N10+O10))))),"",L11+IF(N10="x",IF(AND(P10="x",R10="x"),30,IF(P10="x",20+R10,IF(Q10="/",20,10+P10+Q10))),IF(AND(O10="/",P10="x"),20,IF(O10="/",10+P10,IF(OR((N10+O10)&gt;9,O10=""),"",N10+O10))))),"")</f>
-        <v/>
-      </c>
-      <c r="O11" s="42"/>
-      <c r="P11" s="41" t="str">
+        <v>40</v>
+      </c>
+      <c r="O11" s="44"/>
+      <c r="P11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;""),IF(ISERROR(N11+IF(P10="x",IF(AND(R10="x",T10="x"),30,IF(R10="x",20+T10,IF(S10="/",20,10+R10+S10))),IF(AND(Q10="/",R10="x"),20,IF(Q10="/",10+R10,IF(OR((P10+Q10)&gt;9,Q10=""),"",P10+Q10))))),"",N11+IF(P10="x",IF(AND(R10="x",T10="x"),30,IF(R10="x",20+T10,IF(S10="/",20,10+R10+S10))),IF(AND(Q10="/",R10="x"),20,IF(Q10="/",10+R10,IF(OR((P10+Q10)&gt;9,Q10=""),"",P10+Q10))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="41" t="str">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;"",R10&lt;&gt;""),IF(ISERROR(P11+IF(R10="x",IF(AND(T10="x",U10="x"),30,IF(T10="x",20+U10,IF(U10="/",20,10+T10+U10))),IF(AND(S10="/",T10="x"),20,IF(S10="/",10+T10,IF(OR((R10+S10)&gt;9,S10=""),"",R10+S10))))),"",P11+IF(R10="x",IF(AND(T10="x",U10="x"),30,IF(T10="x",20+U10,IF(U10="/",20,10+T10+U10))),IF(AND(S10="/",T10="x"),20,IF(S10="/",10+T10,IF(OR((R10+S10)&gt;9,S10=""),"",R10+S10))))),"")</f>
-        <v/>
-      </c>
-      <c r="S11" s="42"/>
-      <c r="T11" s="41" t="str">
+        <v>52</v>
+      </c>
+      <c r="S11" s="44"/>
+      <c r="T11" s="43">
         <f>IF(AND(B10&lt;&gt;"",D10&lt;&gt;"",F10&lt;&gt;"",H10&lt;&gt;"",J10&lt;&gt;"",L10&lt;&gt;"",N10&lt;&gt;"",P10&lt;&gt;"",R10&lt;&gt;"",T10&lt;&gt;""),IF(ISERROR(R11+IF(T10="x",IF(AND(U10="x",V10="x"),30,IF(U10="x",20+V10,IF(V10="/",20,IF(V10&gt;(9-U10),"",10+U10+V10)))),IF(AND(U10="/",V10="x"),20,IF(U10="/",10+V10,IF(OR((T10+U10)&gt;9,U10=""),"",T10+U10))))),"",R11+IF(T10="x",IF(AND(U10="x",V10="x"),30,IF(U10="x",20+V10,IF(V10="/",20,IF(V10&gt;(9-U10),"",10+U10+V10)))),IF(AND(U10="/",V10="x"),20,IF(U10="/",10+V10,IF(OR((T10+U10)&gt;9,U10=""),"",T10+U10))))),"")</f>
-        <v/>
-      </c>
-      <c r="U11" s="46"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="U11" s="49"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="42"/>
     </row>
     <row r="12" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="str">
+      <c r="A12" s="52" t="str">
         <f>'Bowling 1'!A12</f>
         <v>Name #6</v>
       </c>
@@ -20089,91 +20382,119 @@
       <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="40">
-        <f>SUM(B13:V13)</f>
-        <v>8</v>
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2</v>
+      </c>
+      <c r="M12" s="8">
+        <v>3</v>
+      </c>
+      <c r="N12" s="8">
+        <v>3</v>
+      </c>
+      <c r="O12" s="8">
+        <v>4</v>
+      </c>
+      <c r="P12" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>4</v>
+      </c>
+      <c r="R12" s="8">
+        <v>3</v>
+      </c>
+      <c r="S12" s="8">
+        <v>3</v>
+      </c>
+      <c r="T12" s="11">
+        <v>2</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="41">
+        <f>T13</f>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="36">
+      <c r="A13" s="53"/>
+      <c r="B13" s="56">
         <f>IF(B12&lt;&gt;"",IF(ISERROR(IF(B12="x",IF(AND(D12="x",F12="x"),30,IF(D12="x",20+F12,IF(E12="/",20,10+D12+E12))),IF(AND(C12="/",D12="x"),20,IF(C12="/",10+D12,IF(OR((B12+C12)&gt;9,C12=""),"",B12+C12))))),"",IF(B12="x",IF(AND(D12="x",F12="x"),30,IF(D12="x",20+F12,IF(E12="/",20,10+D12+E12))),IF(AND(C12="/",D12="x"),20,IF(C12="/",10+D12,IF(OR((B12+C12)&gt;9,C12=""),"",B12+C12))))),"")</f>
         <v>2</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="43">
+      <c r="C13" s="46"/>
+      <c r="D13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;""),IF(ISERROR(B13+IF(D12="x",IF(AND(F12="x",H12="x"),30,IF(F12="x",20+H12,IF(G12="/",20,10+F12+G12))),IF(AND(E12="/",F12="x"),20,IF(E12="/",10+F12,IF(OR((D12+E12)&gt;9,E12=""),"",D12+E12))))),"",B13+IF(D12="x",IF(AND(F12="x",H12="x"),30,IF(F12="x",20+H12,IF(G12="/",20,10+F12+G12))),IF(AND(E12="/",F12="x"),20,IF(E12="/",10+F12,IF(OR((D12+E12)&gt;9,E12=""),"",D12+E12))))),"")</f>
         <v>6</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="43" t="str">
+      <c r="E13" s="46"/>
+      <c r="F13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;""),IF(ISERROR(D13+IF(F12="x",IF(AND(H12="x",J12="x"),30,IF(H12="x",20+J12,IF(I12="/",20,10+H12+I12))),IF(AND(G12="/",H12="x"),20,IF(G12="/",10+H12,IF(OR((F12+G12)&gt;9,G12=""),"",F12+G12))))),"",D13+IF(F12="x",IF(AND(H12="x",J12="x"),30,IF(H12="x",20+J12,IF(I12="/",20,10+H12+I12))),IF(AND(G12="/",H12="x"),20,IF(G12="/",10+H12,IF(OR((F12+G12)&gt;9,G12=""),"",F12+G12))))),"")</f>
-        <v/>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="43" t="str">
+        <v>9</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;""),IF(ISERROR(F13+IF(H12="x",IF(AND(J12="x",L12="x"),30,IF(J12="x",20+L12,IF(K12="/",20,10+J12+K12))),IF(AND(I12="/",J12="x"),20,IF(I12="/",10+J12,IF(OR((H12+I12)&gt;9,I12=""),"",H12+I12))))),"",F13+IF(H12="x",IF(AND(J12="x",L12="x"),30,IF(J12="x",20+L12,IF(K12="/",20,10+J12+K12))),IF(AND(I12="/",J12="x"),20,IF(I12="/",10+J12,IF(OR((H12+I12)&gt;9,I12=""),"",H12+I12))))),"")</f>
-        <v/>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="43" t="str">
+        <v>11</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;""),IF(ISERROR(H13+IF(J12="x",IF(AND(L12="x",N12="x"),30,IF(L12="x",20+N12,IF(M12="/",20,10+L12+M12))),IF(AND(K12="/",L12="x"),20,IF(K12="/",10+L12,IF(OR((J12+K12)&gt;9,K12=""),"",J12+K12))))),"",H13+IF(J12="x",IF(AND(L12="x",N12="x"),30,IF(L12="x",20+N12,IF(M12="/",20,10+L12+M12))),IF(AND(K12="/",L12="x"),20,IF(K12="/",10+L12,IF(OR((J12+K12)&gt;9,K12=""),"",J12+K12))))),"")</f>
-        <v/>
-      </c>
-      <c r="K13" s="37"/>
-      <c r="L13" s="43" t="str">
+        <v>14</v>
+      </c>
+      <c r="K13" s="46"/>
+      <c r="L13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;""),IF(ISERROR(J13+IF(L12="x",IF(AND(N12="x",P12="x"),30,IF(N12="x",20+P12,IF(O12="/",20,10+N12+O12))),IF(AND(M12="/",N12="x"),20,IF(M12="/",10+N12,IF(OR((L12+M12)&gt;9,M12=""),"",L12+M12))))),"",J13+IF(L12="x",IF(AND(N12="x",P12="x"),30,IF(N12="x",20+P12,IF(O12="/",20,10+N12+O12))),IF(AND(M12="/",N12="x"),20,IF(M12="/",10+N12,IF(OR((L12+M12)&gt;9,M12=""),"",L12+M12))))),"")</f>
-        <v/>
-      </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="43" t="str">
+        <v>19</v>
+      </c>
+      <c r="M13" s="46"/>
+      <c r="N13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;""),IF(ISERROR(L13+IF(N12="x",IF(AND(P12="x",R12="x"),30,IF(P12="x",20+R12,IF(Q12="/",20,10+P12+Q12))),IF(AND(O12="/",P12="x"),20,IF(O12="/",10+P12,IF(OR((N12+O12)&gt;9,O12=""),"",N12+O12))))),"",L13+IF(N12="x",IF(AND(P12="x",R12="x"),30,IF(P12="x",20+R12,IF(Q12="/",20,10+P12+Q12))),IF(AND(O12="/",P12="x"),20,IF(O12="/",10+P12,IF(OR((N12+O12)&gt;9,O12=""),"",N12+O12))))),"")</f>
-        <v/>
-      </c>
-      <c r="O13" s="37"/>
-      <c r="P13" s="43" t="str">
+        <v>26</v>
+      </c>
+      <c r="O13" s="46"/>
+      <c r="P13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;""),IF(ISERROR(N13+IF(P12="x",IF(AND(R12="x",T12="x"),30,IF(R12="x",20+T12,IF(S12="/",20,10+R12+S12))),IF(AND(Q12="/",R12="x"),20,IF(Q12="/",10+R12,IF(OR((P12+Q12)&gt;9,Q12=""),"",P12+Q12))))),"",N13+IF(P12="x",IF(AND(R12="x",T12="x"),30,IF(R12="x",20+T12,IF(S12="/",20,10+R12+S12))),IF(AND(Q12="/",R12="x"),20,IF(Q12="/",10+R12,IF(OR((P12+Q12)&gt;9,Q12=""),"",P12+Q12))))),"")</f>
-        <v/>
-      </c>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="43" t="str">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;"",R12&lt;&gt;""),IF(ISERROR(P13+IF(R12="x",IF(AND(T12="x",U12="x"),30,IF(T12="x",20+U12,IF(U12="/",20,10+T12+U12))),IF(AND(S12="/",T12="x"),20,IF(S12="/",10+T12,IF(OR((R12+S12)&gt;9,S12=""),"",R12+S12))))),"",P13+IF(R12="x",IF(AND(T12="x",U12="x"),30,IF(T12="x",20+U12,IF(U12="/",20,10+T12+U12))),IF(AND(S12="/",T12="x"),20,IF(S12="/",10+T12,IF(OR((R12+S12)&gt;9,S12=""),"",R12+S12))))),"")</f>
-        <v/>
-      </c>
-      <c r="S13" s="37"/>
-      <c r="T13" s="43" t="str">
+        <v>40</v>
+      </c>
+      <c r="S13" s="46"/>
+      <c r="T13" s="45">
         <f>IF(AND(B12&lt;&gt;"",D12&lt;&gt;"",F12&lt;&gt;"",H12&lt;&gt;"",J12&lt;&gt;"",L12&lt;&gt;"",N12&lt;&gt;"",P12&lt;&gt;"",R12&lt;&gt;"",T12&lt;&gt;""),IF(ISERROR(R13+IF(T12="x",IF(AND(U12="x",V12="x"),30,IF(U12="x",20+V12,IF(V12="/",20,IF(V12&gt;(9-U12),"",10+U12+V12)))),IF(AND(U12="/",V12="x"),20,IF(U12="/",10+V12,IF(OR((T12+U12)&gt;9,U12=""),"",T12+U12))))),"",R13+IF(T12="x",IF(AND(U12="x",V12="x"),30,IF(U12="x",20+V12,IF(V12="/",20,IF(V12&gt;(9-U12),"",10+U12+V12)))),IF(AND(U12="/",V12="x"),20,IF(U12="/",10+V12,IF(OR((T12+U12)&gt;9,U12=""),"",T12+U12))))),"")</f>
-        <v/>
-      </c>
-      <c r="U13" s="44"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="39"/>
+        <v>60</v>
+      </c>
+      <c r="U13" s="47"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="T11:V11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="W12:W13"/>
     <mergeCell ref="B13:C13"/>
@@ -20182,6 +20503,10 @@
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:V13"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="W10:W11"/>
     <mergeCell ref="B11:C11"/>
@@ -20192,24 +20517,26 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:V11"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="W6:W7"/>
     <mergeCell ref="B7:C7"/>
@@ -20218,12 +20545,14 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:V1"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
@@ -20232,24 +20561,22 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:V5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -20261,7 +20588,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20272,67 +20599,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59">
+      <c r="B1" s="37">
         <v>1</v>
       </c>
-      <c r="C1" s="60">
+      <c r="C1" s="38">
         <v>2</v>
       </c>
-      <c r="D1" s="60">
+      <c r="D1" s="38">
         <v>3</v>
       </c>
-      <c r="E1" s="60">
+      <c r="E1" s="38">
         <v>4</v>
       </c>
-      <c r="F1" s="60">
+      <c r="F1" s="38">
         <v>5</v>
       </c>
-      <c r="G1" s="60">
+      <c r="G1" s="38">
         <v>6</v>
       </c>
-      <c r="H1" s="60">
+      <c r="H1" s="38">
         <v>7</v>
       </c>
-      <c r="I1" s="60">
+      <c r="I1" s="38">
         <v>8</v>
       </c>
-      <c r="J1" s="60">
+      <c r="J1" s="38">
         <v>9</v>
       </c>
-      <c r="K1" s="60">
+      <c r="K1" s="38">
         <v>10</v>
       </c>
-      <c r="L1" s="60">
+      <c r="L1" s="38">
         <v>11</v>
       </c>
-      <c r="M1" s="60">
+      <c r="M1" s="38">
         <v>12</v>
       </c>
-      <c r="N1" s="60">
+      <c r="N1" s="38">
         <v>13</v>
       </c>
-      <c r="O1" s="60">
+      <c r="O1" s="38">
         <v>14</v>
       </c>
-      <c r="P1" s="60">
+      <c r="P1" s="38">
         <v>15</v>
       </c>
-      <c r="Q1" s="60">
+      <c r="Q1" s="38">
         <v>16</v>
       </c>
-      <c r="R1" s="60">
+      <c r="R1" s="38">
         <v>17</v>
       </c>
-      <c r="S1" s="60">
+      <c r="S1" s="38">
         <v>18</v>
       </c>
-      <c r="T1" s="60">
+      <c r="T1" s="38">
         <v>19</v>
       </c>
-      <c r="U1" s="57">
+      <c r="U1" s="35">
         <v>20</v>
       </c>
       <c r="V1" s="34" t="s">
@@ -20340,49 +20667,49 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="39" t="str">
         <f>'Bowling 1'!A2</f>
         <v>Name #1</v>
       </c>
       <c r="B2" s="4">
         <f>'Bowling 1'!B3</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5">
         <f>'Bowling 1'!D3</f>
-        <v>30</v>
-      </c>
-      <c r="D2" s="5" t="str">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5">
         <f>'Bowling 1'!F3</f>
-        <v/>
-      </c>
-      <c r="E2" s="5" t="str">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5">
         <f>'Bowling 1'!H3</f>
-        <v/>
-      </c>
-      <c r="F2" s="5" t="str">
+        <v>58</v>
+      </c>
+      <c r="F2" s="5">
         <f>'Bowling 1'!J3</f>
-        <v/>
-      </c>
-      <c r="G2" s="5" t="str">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5">
         <f>'Bowling 1'!L3</f>
-        <v/>
-      </c>
-      <c r="H2" s="5" t="str">
+        <v>74</v>
+      </c>
+      <c r="H2" s="5">
         <f>'Bowling 1'!N3</f>
-        <v/>
-      </c>
-      <c r="I2" s="5" t="str">
+        <v>82</v>
+      </c>
+      <c r="I2" s="5">
         <f>'Bowling 1'!P3</f>
-        <v/>
-      </c>
-      <c r="J2" s="5" t="str">
+        <v>90</v>
+      </c>
+      <c r="J2" s="5">
         <f>'Bowling 1'!R3</f>
-        <v/>
-      </c>
-      <c r="K2" s="5" t="str">
+        <v>98</v>
+      </c>
+      <c r="K2" s="5">
         <f>'Bowling 1'!T3</f>
-        <v/>
+        <v>106</v>
       </c>
       <c r="L2" s="5">
         <f>'Bowling 2'!B3</f>
@@ -20425,12 +20752,12 @@
         <v>20</v>
       </c>
       <c r="V2" s="23">
-        <f>SUM(B2:U2)</f>
-        <v>160</v>
+        <f t="shared" ref="V2:V7" si="0">SUM(B2:U2)</f>
+        <v>800</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="str">
+      <c r="A3" s="40" t="str">
         <f>'Bowling 1'!A4</f>
         <v>Name #2</v>
       </c>
@@ -20442,37 +20769,37 @@
         <f>'Bowling 1'!D5</f>
         <v>25</v>
       </c>
-      <c r="D3" s="8" t="str">
+      <c r="D3" s="8">
         <f>'Bowling 1'!F5</f>
-        <v/>
-      </c>
-      <c r="E3" s="8" t="str">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8">
         <f>'Bowling 1'!H5</f>
-        <v/>
-      </c>
-      <c r="F3" s="8" t="str">
+        <v>37</v>
+      </c>
+      <c r="F3" s="8">
         <f>'Bowling 1'!J5</f>
-        <v/>
-      </c>
-      <c r="G3" s="8" t="str">
+        <v>43</v>
+      </c>
+      <c r="G3" s="8">
         <f>'Bowling 1'!L5</f>
-        <v/>
-      </c>
-      <c r="H3" s="8" t="str">
+        <v>49</v>
+      </c>
+      <c r="H3" s="8">
         <f>'Bowling 1'!N5</f>
-        <v/>
-      </c>
-      <c r="I3" s="8" t="str">
+        <v>55</v>
+      </c>
+      <c r="I3" s="8">
         <f>'Bowling 1'!P5</f>
-        <v/>
-      </c>
-      <c r="J3" s="8" t="str">
+        <v>61</v>
+      </c>
+      <c r="J3" s="8">
         <f>'Bowling 1'!R5</f>
-        <v/>
-      </c>
-      <c r="K3" s="8" t="str">
+        <v>67</v>
+      </c>
+      <c r="K3" s="8">
         <f>'Bowling 1'!T5</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="L3" s="8">
         <f>'Bowling 2'!B5</f>
@@ -20482,41 +20809,41 @@
         <f>'Bowling 2'!D5</f>
         <v>25</v>
       </c>
-      <c r="N3" s="8" t="str">
+      <c r="N3" s="8">
         <f>'Bowling 2'!F5</f>
-        <v/>
-      </c>
-      <c r="O3" s="8" t="str">
+        <v>29</v>
+      </c>
+      <c r="O3" s="8">
         <f>'Bowling 2'!H5</f>
-        <v/>
-      </c>
-      <c r="P3" s="8" t="str">
+        <v>33</v>
+      </c>
+      <c r="P3" s="8">
         <f>'Bowling 2'!J5</f>
-        <v/>
-      </c>
-      <c r="Q3" s="8" t="str">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="8">
         <f>'Bowling 2'!L5</f>
-        <v/>
-      </c>
-      <c r="R3" s="8" t="str">
+        <v>41</v>
+      </c>
+      <c r="R3" s="8">
         <f>'Bowling 2'!N5</f>
-        <v/>
-      </c>
-      <c r="S3" s="8" t="str">
+        <v>45</v>
+      </c>
+      <c r="S3" s="8">
         <f>'Bowling 2'!P5</f>
-        <v/>
-      </c>
-      <c r="T3" s="8" t="str">
+        <v>49</v>
+      </c>
+      <c r="T3" s="8">
         <f>'Bowling 2'!R5</f>
-        <v/>
-      </c>
-      <c r="U3" s="9" t="str">
+        <v>53</v>
+      </c>
+      <c r="U3" s="9">
         <f>'Bowling 2'!T5</f>
-        <v/>
+        <v>57</v>
       </c>
       <c r="V3" s="24">
-        <f>SUM(B3:U3)</f>
-        <v>82</v>
+        <f t="shared" si="0"/>
+        <v>842</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20530,39 +20857,39 @@
       </c>
       <c r="C4" s="8">
         <f>'Bowling 1'!D7</f>
-        <v>18</v>
-      </c>
-      <c r="D4" s="8" t="str">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8">
         <f>'Bowling 1'!F7</f>
-        <v/>
-      </c>
-      <c r="E4" s="8" t="str">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8">
         <f>'Bowling 1'!H7</f>
-        <v/>
-      </c>
-      <c r="F4" s="8" t="str">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8">
         <f>'Bowling 1'!J7</f>
-        <v/>
-      </c>
-      <c r="G4" s="8" t="str">
+        <v>32</v>
+      </c>
+      <c r="G4" s="8">
         <f>'Bowling 1'!L7</f>
-        <v/>
-      </c>
-      <c r="H4" s="8" t="str">
+        <v>36</v>
+      </c>
+      <c r="H4" s="8">
         <f>'Bowling 1'!N7</f>
-        <v/>
-      </c>
-      <c r="I4" s="8" t="str">
+        <v>40</v>
+      </c>
+      <c r="I4" s="8">
         <f>'Bowling 1'!P7</f>
-        <v/>
-      </c>
-      <c r="J4" s="8" t="str">
+        <v>44</v>
+      </c>
+      <c r="J4" s="8">
         <f>'Bowling 1'!R7</f>
-        <v/>
-      </c>
-      <c r="K4" s="8" t="str">
+        <v>48</v>
+      </c>
+      <c r="K4" s="8">
         <f>'Bowling 1'!T7</f>
-        <v/>
+        <v>52</v>
       </c>
       <c r="L4" s="8">
         <f>'Bowling 2'!B7</f>
@@ -20570,43 +20897,43 @@
       </c>
       <c r="M4" s="8">
         <f>'Bowling 2'!D7</f>
-        <v>18</v>
-      </c>
-      <c r="N4" s="8" t="str">
+        <v>21</v>
+      </c>
+      <c r="N4" s="8">
         <f>'Bowling 2'!F7</f>
-        <v/>
-      </c>
-      <c r="O4" s="8" t="str">
+        <v>27</v>
+      </c>
+      <c r="O4" s="8">
         <f>'Bowling 2'!H7</f>
-        <v/>
-      </c>
-      <c r="P4" s="8" t="str">
+        <v>33</v>
+      </c>
+      <c r="P4" s="8">
         <f>'Bowling 2'!J7</f>
-        <v/>
-      </c>
-      <c r="Q4" s="8" t="str">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="8">
         <f>'Bowling 2'!L7</f>
-        <v/>
-      </c>
-      <c r="R4" s="8" t="str">
+        <v>45</v>
+      </c>
+      <c r="R4" s="8">
         <f>'Bowling 2'!N7</f>
-        <v/>
-      </c>
-      <c r="S4" s="8" t="str">
+        <v>51</v>
+      </c>
+      <c r="S4" s="8">
         <f>'Bowling 2'!P7</f>
-        <v/>
-      </c>
-      <c r="T4" s="8" t="str">
+        <v>57</v>
+      </c>
+      <c r="T4" s="8">
         <f>'Bowling 2'!R7</f>
-        <v/>
-      </c>
-      <c r="U4" s="9" t="str">
+        <v>63</v>
+      </c>
+      <c r="U4" s="9">
         <f>'Bowling 2'!T7</f>
-        <v/>
+        <v>69</v>
       </c>
       <c r="V4" s="24">
-        <f>SUM(B4:U4)</f>
-        <v>52</v>
+        <f t="shared" si="0"/>
+        <v>745</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20622,37 +20949,37 @@
         <f>'Bowling 1'!D9</f>
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="str">
+      <c r="D5" s="8">
         <f>'Bowling 1'!F9</f>
-        <v/>
-      </c>
-      <c r="E5" s="8" t="str">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8">
         <f>'Bowling 1'!H9</f>
-        <v/>
-      </c>
-      <c r="F5" s="8" t="str">
+        <v>26</v>
+      </c>
+      <c r="F5" s="8">
         <f>'Bowling 1'!J9</f>
-        <v/>
-      </c>
-      <c r="G5" s="8" t="str">
+        <v>28</v>
+      </c>
+      <c r="G5" s="8">
         <f>'Bowling 1'!L9</f>
-        <v/>
-      </c>
-      <c r="H5" s="8" t="str">
+        <v>30</v>
+      </c>
+      <c r="H5" s="8">
         <f>'Bowling 1'!N9</f>
-        <v/>
-      </c>
-      <c r="I5" s="8" t="str">
+        <v>32</v>
+      </c>
+      <c r="I5" s="8">
         <f>'Bowling 1'!P9</f>
-        <v/>
-      </c>
-      <c r="J5" s="8" t="str">
+        <v>34</v>
+      </c>
+      <c r="J5" s="8">
         <f>'Bowling 1'!R9</f>
-        <v/>
-      </c>
-      <c r="K5" s="8" t="str">
+        <v>36</v>
+      </c>
+      <c r="K5" s="8">
         <f>'Bowling 1'!T9</f>
-        <v/>
+        <v>38</v>
       </c>
       <c r="L5" s="8">
         <f>'Bowling 2'!B9</f>
@@ -20662,41 +20989,41 @@
         <f>'Bowling 2'!D9</f>
         <v>14</v>
       </c>
-      <c r="N5" s="8" t="str">
+      <c r="N5" s="8">
         <f>'Bowling 2'!F9</f>
-        <v/>
-      </c>
-      <c r="O5" s="8" t="str">
+        <v>22</v>
+      </c>
+      <c r="O5" s="8">
         <f>'Bowling 2'!H9</f>
-        <v/>
-      </c>
-      <c r="P5" s="8" t="str">
+        <v>30</v>
+      </c>
+      <c r="P5" s="8">
         <f>'Bowling 2'!J9</f>
-        <v/>
-      </c>
-      <c r="Q5" s="8" t="str">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="8">
         <f>'Bowling 2'!L9</f>
-        <v/>
-      </c>
-      <c r="R5" s="8" t="str">
+        <v>46</v>
+      </c>
+      <c r="R5" s="8">
         <f>'Bowling 2'!N9</f>
-        <v/>
-      </c>
-      <c r="S5" s="8" t="str">
+        <v>54</v>
+      </c>
+      <c r="S5" s="8">
         <f>'Bowling 2'!P9</f>
-        <v/>
-      </c>
-      <c r="T5" s="8" t="str">
+        <v>62</v>
+      </c>
+      <c r="T5" s="8">
         <f>'Bowling 2'!R9</f>
-        <v/>
-      </c>
-      <c r="U5" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="U5" s="9">
         <f>'Bowling 2'!T9</f>
-        <v/>
+        <v>78</v>
       </c>
       <c r="V5" s="24">
-        <f>SUM(B5:U5)</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>685</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20752,41 +21079,41 @@
         <f>'Bowling 2'!D11</f>
         <v>10</v>
       </c>
-      <c r="N6" s="8" t="str">
+      <c r="N6" s="8">
         <f>'Bowling 2'!F11</f>
-        <v/>
-      </c>
-      <c r="O6" s="8" t="str">
+        <v>16</v>
+      </c>
+      <c r="O6" s="8">
         <f>'Bowling 2'!H11</f>
-        <v/>
-      </c>
-      <c r="P6" s="8" t="str">
+        <v>22</v>
+      </c>
+      <c r="P6" s="8">
         <f>'Bowling 2'!J11</f>
-        <v/>
-      </c>
-      <c r="Q6" s="8" t="str">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="8">
         <f>'Bowling 2'!L11</f>
-        <v/>
-      </c>
-      <c r="R6" s="8" t="str">
+        <v>34</v>
+      </c>
+      <c r="R6" s="8">
         <f>'Bowling 2'!N11</f>
-        <v/>
-      </c>
-      <c r="S6" s="8" t="str">
+        <v>40</v>
+      </c>
+      <c r="S6" s="8">
         <f>'Bowling 2'!P11</f>
-        <v/>
-      </c>
-      <c r="T6" s="8" t="str">
+        <v>46</v>
+      </c>
+      <c r="T6" s="8">
         <f>'Bowling 2'!R11</f>
-        <v/>
-      </c>
-      <c r="U6" s="9" t="str">
+        <v>52</v>
+      </c>
+      <c r="U6" s="9">
         <f>'Bowling 2'!T11</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="V6" s="24">
-        <f>SUM(B6:U6)</f>
-        <v>180</v>
+        <f t="shared" si="0"/>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20802,37 +21129,37 @@
         <f>'Bowling 1'!D13</f>
         <v>6</v>
       </c>
-      <c r="D7" s="11" t="str">
+      <c r="D7" s="11">
         <f>'Bowling 1'!F13</f>
-        <v/>
-      </c>
-      <c r="E7" s="11" t="str">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11">
         <f>'Bowling 1'!H13</f>
-        <v/>
-      </c>
-      <c r="F7" s="11" t="str">
+        <v>22</v>
+      </c>
+      <c r="F7" s="11">
         <f>'Bowling 1'!J13</f>
-        <v/>
-      </c>
-      <c r="G7" s="11" t="str">
+        <v>27</v>
+      </c>
+      <c r="G7" s="11">
         <f>'Bowling 1'!L13</f>
-        <v/>
-      </c>
-      <c r="H7" s="11" t="str">
+        <v>32</v>
+      </c>
+      <c r="H7" s="11">
         <f>'Bowling 1'!N13</f>
-        <v/>
-      </c>
-      <c r="I7" s="11" t="str">
+        <v>36</v>
+      </c>
+      <c r="I7" s="11">
         <f>'Bowling 1'!P13</f>
-        <v/>
-      </c>
-      <c r="J7" s="11" t="str">
+        <v>43</v>
+      </c>
+      <c r="J7" s="11">
         <f>'Bowling 1'!R13</f>
-        <v/>
-      </c>
-      <c r="K7" s="11" t="str">
+        <v>52</v>
+      </c>
+      <c r="K7" s="11">
         <f>'Bowling 1'!T13</f>
-        <v/>
+        <v>68</v>
       </c>
       <c r="L7" s="11">
         <f>'Bowling 2'!B13</f>
@@ -20842,41 +21169,41 @@
         <f>'Bowling 2'!D13</f>
         <v>6</v>
       </c>
-      <c r="N7" s="11" t="str">
+      <c r="N7" s="11">
         <f>'Bowling 2'!F13</f>
-        <v/>
-      </c>
-      <c r="O7" s="11" t="str">
+        <v>9</v>
+      </c>
+      <c r="O7" s="11">
         <f>'Bowling 2'!H13</f>
-        <v/>
-      </c>
-      <c r="P7" s="11" t="str">
+        <v>11</v>
+      </c>
+      <c r="P7" s="11">
         <f>'Bowling 2'!J13</f>
-        <v/>
-      </c>
-      <c r="Q7" s="11" t="str">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="11">
         <f>'Bowling 2'!L13</f>
-        <v/>
-      </c>
-      <c r="R7" s="11" t="str">
+        <v>19</v>
+      </c>
+      <c r="R7" s="11">
         <f>'Bowling 2'!N13</f>
-        <v/>
-      </c>
-      <c r="S7" s="11" t="str">
+        <v>26</v>
+      </c>
+      <c r="S7" s="11">
         <f>'Bowling 2'!P13</f>
-        <v/>
-      </c>
-      <c r="T7" s="11" t="str">
+        <v>34</v>
+      </c>
+      <c r="T7" s="11">
         <f>'Bowling 2'!R13</f>
-        <v/>
-      </c>
-      <c r="U7" s="12" t="str">
+        <v>40</v>
+      </c>
+      <c r="U7" s="12">
         <f>'Bowling 2'!T13</f>
-        <v/>
+        <v>60</v>
       </c>
       <c r="V7" s="25">
-        <f>SUM(B7:U7)</f>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>